<commit_message>
Added new file GDB_tracepoints.xls, list_file_git.txt. Modified my_scripts/.bash_aliases, buildmfp.sh, git_noted.txt
</commit_message>
<xml_diff>
--- a/List_Tasks_Doing.xlsx
+++ b/List_Tasks_Doing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7995" tabRatio="666" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7995" tabRatio="666"/>
   </bookViews>
   <sheets>
     <sheet name="2Portlan" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,13 @@
     <sheet name="No56_MediaMapFile" sheetId="15" state="hidden" r:id="rId8"/>
     <sheet name="No81_SipSDK" sheetId="17" state="hidden" r:id="rId9"/>
     <sheet name="No52_AirPressureSensor" sheetId="18" state="hidden" r:id="rId10"/>
-    <sheet name="ARM8Soc_Inves" sheetId="20" state="hidden" r:id="rId11"/>
+    <sheet name="ARM8Soc_Inves" sheetId="20" r:id="rId11"/>
     <sheet name="RQ-475" sheetId="21" state="hidden" r:id="rId12"/>
     <sheet name="RQ-571_UT" sheetId="22" state="hidden" r:id="rId13"/>
     <sheet name="RQ-686_UT_SMB" sheetId="24" state="hidden" r:id="rId14"/>
     <sheet name="No44_Dipsw_Inves" sheetId="23" state="hidden" r:id="rId15"/>
-    <sheet name="Sparrow_No22_No23" sheetId="25" r:id="rId16"/>
-    <sheet name="Eagle_No.103" sheetId="26" r:id="rId17"/>
+    <sheet name="Sparrow_No22_No23" sheetId="25" state="hidden" r:id="rId16"/>
+    <sheet name="Eagle_No.103" sheetId="26" state="hidden" r:id="rId17"/>
     <sheet name="HDD_Data_Backup" sheetId="27" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="1315">
   <si>
     <t>APIC_MailSendSetting</t>
   </si>
@@ -5302,6 +5302,20 @@
   </si>
   <si>
     <t>Find machine_type QT_Version</t>
+  </si>
+  <si>
+    <t>./api/jobspec/inc/typs_cpp_jobspec_common.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5023 // 2017.7.25 IT5_4.2 RQ-686 複合機の複数ネットワーク対応 s.yagi Start.
+ 5024 //概要　　：ネットワーク指定.
+ 5025 typedef uchar TYPE_NetworkSpecific;
+ 5026     #define TYPE_NetworkSpecific_NW1        0       ///&lt; ネットワーク1.
+ 5027     #define TYPE_NetworkSpecific_NW2        1       ///&lt; ネットワーク2.
+ 5028     #define TYPE_NetworkSpecific_MAX        2       ///&lt; 最大値.
+ 5029     #define TYPE_NetworkSpecific_ALL        254     ///&lt; 全ネットワーク指定.
+ 5030     #define TYPE_NetworkSpecific_NONE       255     ///&lt; 未指定.
+ 5031 // 2017.7.25 IT5_4.2 RQ-686 複合機の複数ネットワーク対応 s.yagi End.</t>
   </si>
 </sst>
 </file>
@@ -5653,6 +5667,8 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6291,19 +6307,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6313,13 +6317,13 @@
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="5" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6333,8 +6337,20 @@
     <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6650,10 +6666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6923,6 +6939,14 @@
       </c>
       <c r="C43" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="240">
+      <c r="A47" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>1314</v>
       </c>
     </row>
   </sheetData>
@@ -8625,7 +8649,7 @@
   <dimension ref="B4:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8676,7 +8700,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11226,7 +11250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
@@ -11609,7 +11633,7 @@
   <dimension ref="A1:S104"/>
   <sheetViews>
     <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12388,147 +12412,147 @@
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="103" t="s">
         <v>474</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="104" t="s">
         <v>475</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="96" t="s">
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="92" t="s">
         <v>476</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="96" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="92" t="s">
         <v>477</v>
       </c>
-      <c r="H2" s="97"/>
+      <c r="H2" s="93"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="101" t="s">
         <v>478</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="98">
-        <v>1</v>
-      </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98">
-        <v>1</v>
-      </c>
-      <c r="H3" s="98"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="91">
+        <v>1</v>
+      </c>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91">
+        <v>1</v>
+      </c>
+      <c r="H3" s="91"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="101" t="s">
         <v>479</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="98">
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="91">
         <v>2</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98">
+      <c r="F4" s="91"/>
+      <c r="G4" s="91">
         <v>2</v>
       </c>
-      <c r="H4" s="98"/>
+      <c r="H4" s="91"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="101" t="s">
         <v>480</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="98">
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="91">
         <v>4</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98">
+      <c r="F5" s="91"/>
+      <c r="G5" s="91">
         <v>4</v>
       </c>
-      <c r="H5" s="98"/>
+      <c r="H5" s="91"/>
     </row>
     <row r="6" spans="1:31">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="101" t="s">
         <v>481</v>
       </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="99">
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="96">
         <v>8</v>
       </c>
-      <c r="F6" s="99"/>
-      <c r="G6" s="98">
+      <c r="F6" s="96"/>
+      <c r="G6" s="91">
         <v>4</v>
       </c>
-      <c r="H6" s="98"/>
+      <c r="H6" s="91"/>
     </row>
     <row r="7" spans="1:31">
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="101" t="s">
         <v>482</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="98">
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="91">
         <v>8</v>
       </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98">
+      <c r="F7" s="91"/>
+      <c r="G7" s="91">
         <v>8</v>
       </c>
-      <c r="H7" s="98"/>
+      <c r="H7" s="91"/>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="101" t="s">
         <v>483</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="98">
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="91">
         <v>4</v>
       </c>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98">
+      <c r="F8" s="91"/>
+      <c r="G8" s="91">
         <v>4</v>
       </c>
-      <c r="H8" s="98"/>
+      <c r="H8" s="91"/>
     </row>
     <row r="9" spans="1:31">
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="101" t="s">
         <v>484</v>
       </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="98">
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="91">
         <v>8</v>
       </c>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98">
+      <c r="F9" s="91"/>
+      <c r="G9" s="91">
         <v>8</v>
       </c>
-      <c r="H9" s="98"/>
+      <c r="H9" s="91"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="101" t="s">
         <v>485</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="99">
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="96">
         <v>8</v>
       </c>
-      <c r="F10" s="99"/>
-      <c r="G10" s="98">
+      <c r="F10" s="96"/>
+      <c r="G10" s="91">
         <v>4</v>
       </c>
-      <c r="H10" s="98"/>
+      <c r="H10" s="91"/>
     </row>
     <row r="13" spans="1:31" ht="15.75">
       <c r="A13" s="28" t="s">
@@ -12821,12 +12845,12 @@
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
-      <c r="H23" s="101" t="s">
+      <c r="H23" s="97" t="s">
         <v>474</v>
       </c>
-      <c r="I23" s="102"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="103"/>
+      <c r="I23" s="98"/>
+      <c r="J23" s="98"/>
+      <c r="K23" s="99"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
@@ -12849,512 +12873,559 @@
       <c r="AE23" s="26"/>
     </row>
     <row r="24" spans="1:33">
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="100" t="s">
         <v>475</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="96" t="s">
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="92" t="s">
         <v>476</v>
       </c>
-      <c r="I24" s="97"/>
-      <c r="J24" s="96" t="s">
+      <c r="I24" s="93"/>
+      <c r="J24" s="92" t="s">
         <v>477</v>
       </c>
-      <c r="K24" s="97"/>
-      <c r="L24" s="105" t="s">
+      <c r="K24" s="93"/>
+      <c r="L24" s="95" t="s">
         <v>495</v>
       </c>
-      <c r="M24" s="105"/>
-      <c r="N24" s="105"/>
-      <c r="O24" s="105"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="105"/>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
-      <c r="W24" s="105"/>
-      <c r="X24" s="105"/>
-      <c r="Y24" s="105"/>
-      <c r="Z24" s="105"/>
-      <c r="AA24" s="105"/>
-      <c r="AB24" s="105"/>
-      <c r="AC24" s="105"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="105"/>
+      <c r="M24" s="95"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="95"/>
+      <c r="U24" s="95"/>
+      <c r="V24" s="95"/>
+      <c r="W24" s="95"/>
+      <c r="X24" s="95"/>
+      <c r="Y24" s="95"/>
+      <c r="Z24" s="95"/>
+      <c r="AA24" s="95"/>
+      <c r="AB24" s="95"/>
+      <c r="AC24" s="95"/>
+      <c r="AD24" s="95"/>
+      <c r="AE24" s="95"/>
     </row>
     <row r="25" spans="1:33">
-      <c r="B25" s="100" t="s">
+      <c r="B25" s="94" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="100"/>
-      <c r="H25" s="98">
-        <v>1</v>
-      </c>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98">
-        <v>1</v>
-      </c>
-      <c r="K25" s="98"/>
-      <c r="L25" s="100" t="s">
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="91">
+        <v>1</v>
+      </c>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91">
+        <v>1</v>
+      </c>
+      <c r="K25" s="91"/>
+      <c r="L25" s="94" t="s">
         <v>497</v>
       </c>
-      <c r="M25" s="100"/>
-      <c r="N25" s="100"/>
-      <c r="O25" s="100"/>
-      <c r="P25" s="100"/>
-      <c r="Q25" s="100"/>
-      <c r="R25" s="100"/>
-      <c r="S25" s="100"/>
-      <c r="T25" s="100"/>
-      <c r="U25" s="100"/>
-      <c r="V25" s="100"/>
-      <c r="W25" s="100"/>
-      <c r="X25" s="100"/>
-      <c r="Y25" s="100"/>
-      <c r="Z25" s="100"/>
-      <c r="AA25" s="100"/>
-      <c r="AB25" s="100"/>
-      <c r="AC25" s="100"/>
-      <c r="AD25" s="100"/>
-      <c r="AE25" s="100"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="94"/>
+      <c r="O25" s="94"/>
+      <c r="P25" s="94"/>
+      <c r="Q25" s="94"/>
+      <c r="R25" s="94"/>
+      <c r="S25" s="94"/>
+      <c r="T25" s="94"/>
+      <c r="U25" s="94"/>
+      <c r="V25" s="94"/>
+      <c r="W25" s="94"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="94"/>
+      <c r="Z25" s="94"/>
+      <c r="AA25" s="94"/>
+      <c r="AB25" s="94"/>
+      <c r="AC25" s="94"/>
+      <c r="AD25" s="94"/>
+      <c r="AE25" s="94"/>
     </row>
     <row r="26" spans="1:33">
-      <c r="B26" s="100" t="s">
+      <c r="B26" s="94" t="s">
         <v>498</v>
       </c>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="98">
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="94"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="91">
         <v>2</v>
       </c>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98">
+      <c r="I26" s="91"/>
+      <c r="J26" s="91">
         <v>2</v>
       </c>
-      <c r="K26" s="98"/>
-      <c r="L26" s="100" t="s">
+      <c r="K26" s="91"/>
+      <c r="L26" s="94" t="s">
         <v>499</v>
       </c>
-      <c r="M26" s="100"/>
-      <c r="N26" s="100"/>
-      <c r="O26" s="100"/>
-      <c r="P26" s="100"/>
-      <c r="Q26" s="100"/>
-      <c r="R26" s="100"/>
-      <c r="S26" s="100"/>
-      <c r="T26" s="100"/>
-      <c r="U26" s="100"/>
-      <c r="V26" s="100"/>
-      <c r="W26" s="100"/>
-      <c r="X26" s="100"/>
-      <c r="Y26" s="100"/>
-      <c r="Z26" s="100"/>
-      <c r="AA26" s="100"/>
-      <c r="AB26" s="100"/>
-      <c r="AC26" s="100"/>
-      <c r="AD26" s="100"/>
-      <c r="AE26" s="100"/>
+      <c r="M26" s="94"/>
+      <c r="N26" s="94"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="94"/>
+      <c r="R26" s="94"/>
+      <c r="S26" s="94"/>
+      <c r="T26" s="94"/>
+      <c r="U26" s="94"/>
+      <c r="V26" s="94"/>
+      <c r="W26" s="94"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="94"/>
+      <c r="Z26" s="94"/>
+      <c r="AA26" s="94"/>
+      <c r="AB26" s="94"/>
+      <c r="AC26" s="94"/>
+      <c r="AD26" s="94"/>
+      <c r="AE26" s="94"/>
     </row>
     <row r="27" spans="1:33">
-      <c r="B27" s="100" t="s">
+      <c r="B27" s="94" t="s">
         <v>500</v>
       </c>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="98">
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="91">
         <v>4</v>
       </c>
-      <c r="I27" s="98"/>
-      <c r="J27" s="98">
+      <c r="I27" s="91"/>
+      <c r="J27" s="91">
         <v>4</v>
       </c>
-      <c r="K27" s="98"/>
-      <c r="L27" s="100" t="s">
+      <c r="K27" s="91"/>
+      <c r="L27" s="94" t="s">
         <v>501</v>
       </c>
-      <c r="M27" s="100"/>
-      <c r="N27" s="100"/>
-      <c r="O27" s="100"/>
-      <c r="P27" s="100"/>
-      <c r="Q27" s="100"/>
-      <c r="R27" s="100"/>
-      <c r="S27" s="100"/>
-      <c r="T27" s="100"/>
-      <c r="U27" s="100"/>
-      <c r="V27" s="100"/>
-      <c r="W27" s="100"/>
-      <c r="X27" s="100"/>
-      <c r="Y27" s="100"/>
-      <c r="Z27" s="100"/>
-      <c r="AA27" s="100"/>
-      <c r="AB27" s="100"/>
-      <c r="AC27" s="100"/>
-      <c r="AD27" s="100"/>
-      <c r="AE27" s="100"/>
+      <c r="M27" s="94"/>
+      <c r="N27" s="94"/>
+      <c r="O27" s="94"/>
+      <c r="P27" s="94"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="94"/>
+      <c r="T27" s="94"/>
+      <c r="U27" s="94"/>
+      <c r="V27" s="94"/>
+      <c r="W27" s="94"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="94"/>
+      <c r="Z27" s="94"/>
+      <c r="AA27" s="94"/>
+      <c r="AB27" s="94"/>
+      <c r="AC27" s="94"/>
+      <c r="AD27" s="94"/>
+      <c r="AE27" s="94"/>
     </row>
     <row r="28" spans="1:33">
-      <c r="B28" s="100" t="s">
+      <c r="B28" s="94" t="s">
         <v>502</v>
       </c>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="98">
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="91">
         <v>4</v>
       </c>
-      <c r="I28" s="98"/>
-      <c r="J28" s="98">
+      <c r="I28" s="91"/>
+      <c r="J28" s="91">
         <v>4</v>
       </c>
-      <c r="K28" s="98"/>
-      <c r="L28" s="100" t="s">
+      <c r="K28" s="91"/>
+      <c r="L28" s="94" t="s">
         <v>503</v>
       </c>
-      <c r="M28" s="100"/>
-      <c r="N28" s="100"/>
-      <c r="O28" s="100"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="100"/>
-      <c r="R28" s="100"/>
-      <c r="S28" s="100"/>
-      <c r="T28" s="100"/>
-      <c r="U28" s="100"/>
-      <c r="V28" s="100"/>
-      <c r="W28" s="100"/>
-      <c r="X28" s="100"/>
-      <c r="Y28" s="100"/>
-      <c r="Z28" s="100"/>
-      <c r="AA28" s="100"/>
-      <c r="AB28" s="100"/>
-      <c r="AC28" s="100"/>
-      <c r="AD28" s="100"/>
-      <c r="AE28" s="100"/>
+      <c r="M28" s="94"/>
+      <c r="N28" s="94"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="94"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="94"/>
+      <c r="V28" s="94"/>
+      <c r="W28" s="94"/>
+      <c r="X28" s="94"/>
+      <c r="Y28" s="94"/>
+      <c r="Z28" s="94"/>
+      <c r="AA28" s="94"/>
+      <c r="AB28" s="94"/>
+      <c r="AC28" s="94"/>
+      <c r="AD28" s="94"/>
+      <c r="AE28" s="94"/>
     </row>
     <row r="29" spans="1:33">
-      <c r="B29" s="100" t="s">
+      <c r="B29" s="94" t="s">
         <v>504</v>
       </c>
-      <c r="C29" s="100"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="100"/>
-      <c r="H29" s="98">
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="91">
         <v>8</v>
       </c>
-      <c r="I29" s="98"/>
-      <c r="J29" s="98">
+      <c r="I29" s="91"/>
+      <c r="J29" s="91">
         <v>8</v>
       </c>
-      <c r="K29" s="98"/>
-      <c r="L29" s="100" t="s">
+      <c r="K29" s="91"/>
+      <c r="L29" s="94" t="s">
         <v>505</v>
       </c>
-      <c r="M29" s="100"/>
-      <c r="N29" s="100"/>
-      <c r="O29" s="100"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
-      <c r="S29" s="100"/>
-      <c r="T29" s="100"/>
-      <c r="U29" s="100"/>
-      <c r="V29" s="100"/>
-      <c r="W29" s="100"/>
-      <c r="X29" s="100"/>
-      <c r="Y29" s="100"/>
-      <c r="Z29" s="100"/>
-      <c r="AA29" s="100"/>
-      <c r="AB29" s="100"/>
-      <c r="AC29" s="100"/>
-      <c r="AD29" s="100"/>
-      <c r="AE29" s="100"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="94"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="26"/>
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="94" t="s">
         <v>506</v>
       </c>
-      <c r="C30" s="100"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="100"/>
-      <c r="H30" s="99">
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="96">
         <v>8</v>
       </c>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99">
+      <c r="I30" s="96"/>
+      <c r="J30" s="96">
         <v>4</v>
       </c>
-      <c r="K30" s="99"/>
-      <c r="L30" s="100" t="s">
+      <c r="K30" s="96"/>
+      <c r="L30" s="94" t="s">
         <v>507</v>
       </c>
-      <c r="M30" s="100"/>
-      <c r="N30" s="100"/>
-      <c r="O30" s="100"/>
-      <c r="P30" s="100"/>
-      <c r="Q30" s="100"/>
-      <c r="R30" s="100"/>
-      <c r="S30" s="100"/>
-      <c r="T30" s="100"/>
-      <c r="U30" s="100"/>
-      <c r="V30" s="100"/>
-      <c r="W30" s="100"/>
-      <c r="X30" s="100"/>
-      <c r="Y30" s="100"/>
-      <c r="Z30" s="100"/>
-      <c r="AA30" s="100"/>
-      <c r="AB30" s="100"/>
-      <c r="AC30" s="100"/>
-      <c r="AD30" s="100"/>
-      <c r="AE30" s="100"/>
+      <c r="M30" s="94"/>
+      <c r="N30" s="94"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="94"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="94"/>
+      <c r="X30" s="94"/>
+      <c r="Y30" s="94"/>
+      <c r="Z30" s="94"/>
+      <c r="AA30" s="94"/>
+      <c r="AB30" s="94"/>
+      <c r="AC30" s="94"/>
+      <c r="AD30" s="94"/>
+      <c r="AE30" s="94"/>
       <c r="AF30" s="26"/>
       <c r="AG30" s="26"/>
     </row>
     <row r="31" spans="1:33">
       <c r="A31" s="26"/>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="94" t="s">
         <v>508</v>
       </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="99">
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="96">
         <v>8</v>
       </c>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99">
+      <c r="I31" s="96"/>
+      <c r="J31" s="96">
         <v>4</v>
       </c>
-      <c r="K31" s="99"/>
-      <c r="L31" s="100" t="s">
+      <c r="K31" s="96"/>
+      <c r="L31" s="94" t="s">
         <v>509</v>
       </c>
-      <c r="M31" s="100"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="100"/>
-      <c r="S31" s="100"/>
-      <c r="T31" s="100"/>
-      <c r="U31" s="100"/>
-      <c r="V31" s="100"/>
-      <c r="W31" s="100"/>
-      <c r="X31" s="100"/>
-      <c r="Y31" s="100"/>
-      <c r="Z31" s="100"/>
-      <c r="AA31" s="100"/>
-      <c r="AB31" s="100"/>
-      <c r="AC31" s="100"/>
-      <c r="AD31" s="100"/>
-      <c r="AE31" s="100"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="94"/>
+      <c r="X31" s="94"/>
+      <c r="Y31" s="94"/>
+      <c r="Z31" s="94"/>
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="94"/>
+      <c r="AC31" s="94"/>
+      <c r="AD31" s="94"/>
+      <c r="AE31" s="94"/>
       <c r="AF31" s="26"/>
       <c r="AG31" s="26"/>
     </row>
     <row r="32" spans="1:33">
       <c r="A32" s="26"/>
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="94" t="s">
         <v>483</v>
       </c>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="98">
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="91">
         <v>4</v>
       </c>
-      <c r="I32" s="98"/>
-      <c r="J32" s="98">
+      <c r="I32" s="91"/>
+      <c r="J32" s="91">
         <v>4</v>
       </c>
-      <c r="K32" s="98"/>
-      <c r="L32" s="100" t="s">
+      <c r="K32" s="91"/>
+      <c r="L32" s="94" t="s">
         <v>510</v>
       </c>
-      <c r="M32" s="100"/>
-      <c r="N32" s="100"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="100"/>
-      <c r="Q32" s="100"/>
-      <c r="R32" s="100"/>
-      <c r="S32" s="100"/>
-      <c r="T32" s="100"/>
-      <c r="U32" s="100"/>
-      <c r="V32" s="100"/>
-      <c r="W32" s="100"/>
-      <c r="X32" s="100"/>
-      <c r="Y32" s="100"/>
-      <c r="Z32" s="100"/>
-      <c r="AA32" s="100"/>
-      <c r="AB32" s="100"/>
-      <c r="AC32" s="100"/>
-      <c r="AD32" s="100"/>
-      <c r="AE32" s="100"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
+      <c r="V32" s="94"/>
+      <c r="W32" s="94"/>
+      <c r="X32" s="94"/>
+      <c r="Y32" s="94"/>
+      <c r="Z32" s="94"/>
+      <c r="AA32" s="94"/>
+      <c r="AB32" s="94"/>
+      <c r="AC32" s="94"/>
+      <c r="AD32" s="94"/>
+      <c r="AE32" s="94"/>
       <c r="AF32" s="26"/>
       <c r="AG32" s="26"/>
     </row>
     <row r="33" spans="1:33">
       <c r="A33" s="26"/>
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="94" t="s">
         <v>484</v>
       </c>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="98">
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="91">
         <v>8</v>
       </c>
-      <c r="I33" s="98"/>
-      <c r="J33" s="98">
+      <c r="I33" s="91"/>
+      <c r="J33" s="91">
         <v>8</v>
       </c>
-      <c r="K33" s="98"/>
-      <c r="L33" s="100" t="s">
+      <c r="K33" s="91"/>
+      <c r="L33" s="94" t="s">
         <v>511</v>
       </c>
-      <c r="M33" s="100"/>
-      <c r="N33" s="100"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="100"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="100"/>
-      <c r="S33" s="100"/>
-      <c r="T33" s="100"/>
-      <c r="U33" s="100"/>
-      <c r="V33" s="100"/>
-      <c r="W33" s="100"/>
-      <c r="X33" s="100"/>
-      <c r="Y33" s="100"/>
-      <c r="Z33" s="100"/>
-      <c r="AA33" s="100"/>
-      <c r="AB33" s="100"/>
-      <c r="AC33" s="100"/>
-      <c r="AD33" s="100"/>
-      <c r="AE33" s="100"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="94"/>
       <c r="AF33" s="26"/>
       <c r="AG33" s="26"/>
     </row>
     <row r="34" spans="1:33">
       <c r="A34" s="26"/>
-      <c r="B34" s="100" t="s">
+      <c r="B34" s="94" t="s">
         <v>512</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-      <c r="H34" s="98">
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="91">
         <v>8</v>
       </c>
-      <c r="I34" s="98"/>
-      <c r="J34" s="98">
+      <c r="I34" s="91"/>
+      <c r="J34" s="91">
         <v>8</v>
       </c>
-      <c r="K34" s="98"/>
-      <c r="L34" s="100" t="s">
+      <c r="K34" s="91"/>
+      <c r="L34" s="94" t="s">
         <v>505</v>
       </c>
-      <c r="M34" s="100"/>
-      <c r="N34" s="100"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="100"/>
-      <c r="Q34" s="100"/>
-      <c r="R34" s="100"/>
-      <c r="S34" s="100"/>
-      <c r="T34" s="100"/>
-      <c r="U34" s="100"/>
-      <c r="V34" s="100"/>
-      <c r="W34" s="100"/>
-      <c r="X34" s="100"/>
-      <c r="Y34" s="100"/>
-      <c r="Z34" s="100"/>
-      <c r="AA34" s="100"/>
-      <c r="AB34" s="100"/>
-      <c r="AC34" s="100"/>
-      <c r="AD34" s="100"/>
-      <c r="AE34" s="100"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="94"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="94"/>
+      <c r="Q34" s="94"/>
+      <c r="R34" s="94"/>
+      <c r="S34" s="94"/>
+      <c r="T34" s="94"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="94"/>
+      <c r="Y34" s="94"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="94"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="94"/>
+      <c r="AE34" s="94"/>
       <c r="AF34" s="26"/>
       <c r="AG34" s="26"/>
     </row>
     <row r="35" spans="1:33">
       <c r="A35" s="26"/>
-      <c r="B35" s="100" t="s">
+      <c r="B35" s="94" t="s">
         <v>513</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="99">
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="96">
         <v>8</v>
       </c>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99">
+      <c r="I35" s="96"/>
+      <c r="J35" s="96">
         <v>4</v>
       </c>
-      <c r="K35" s="99"/>
-      <c r="L35" s="100" t="s">
+      <c r="K35" s="96"/>
+      <c r="L35" s="94" t="s">
         <v>514</v>
       </c>
-      <c r="M35" s="100"/>
-      <c r="N35" s="100"/>
-      <c r="O35" s="100"/>
-      <c r="P35" s="100"/>
-      <c r="Q35" s="100"/>
-      <c r="R35" s="100"/>
-      <c r="S35" s="100"/>
-      <c r="T35" s="100"/>
-      <c r="U35" s="100"/>
-      <c r="V35" s="100"/>
-      <c r="W35" s="100"/>
-      <c r="X35" s="100"/>
-      <c r="Y35" s="100"/>
-      <c r="Z35" s="100"/>
-      <c r="AA35" s="100"/>
-      <c r="AB35" s="100"/>
-      <c r="AC35" s="100"/>
-      <c r="AD35" s="100"/>
-      <c r="AE35" s="100"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="94"/>
+      <c r="AB35" s="94"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="94"/>
       <c r="AF35" s="26"/>
       <c r="AG35" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L25:AE25"/>
-    <mergeCell ref="L24:AE24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="L31:AE31"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="L30:AE30"/>
+    <mergeCell ref="L32:AE32"/>
+    <mergeCell ref="L28:AE28"/>
+    <mergeCell ref="L33:AE33"/>
+    <mergeCell ref="L34:AE34"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="L29:AE29"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
     <mergeCell ref="L35:AE35"/>
     <mergeCell ref="L27:AE27"/>
     <mergeCell ref="L26:AE26"/>
@@ -13371,60 +13442,13 @@
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="B35:G35"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="L31:AE31"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="L30:AE30"/>
-    <mergeCell ref="L32:AE32"/>
-    <mergeCell ref="L28:AE28"/>
-    <mergeCell ref="L33:AE33"/>
-    <mergeCell ref="L34:AE34"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="L29:AE29"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L25:AE25"/>
+    <mergeCell ref="L24:AE24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13745,8 +13769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updadted old files and added new file  my_scripts/buildServer.sh
</commit_message>
<xml_diff>
--- a/List_Tasks_Doing.xlsx
+++ b/List_Tasks_Doing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7995" tabRatio="666" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7995" tabRatio="666" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="2Portlan" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
     <sheet name="No81_SipSDK" sheetId="17" state="hidden" r:id="rId10"/>
     <sheet name="No52_AirPressureSensor" sheetId="18" state="hidden" r:id="rId11"/>
     <sheet name="ARM8Soc_Inves" sheetId="20" r:id="rId12"/>
-    <sheet name="RQ-475" sheetId="21" state="hidden" r:id="rId13"/>
-    <sheet name="RQ-571_UT" sheetId="22" state="hidden" r:id="rId14"/>
+    <sheet name="RQ-475" sheetId="21" r:id="rId13"/>
+    <sheet name="RQ-571_UT" sheetId="22" r:id="rId14"/>
     <sheet name="RQ-686_UT_SMB" sheetId="24" state="hidden" r:id="rId15"/>
     <sheet name="No44_Dipsw_Inves" sheetId="23" state="hidden" r:id="rId16"/>
     <sheet name="Sparrow_No22_No23" sheetId="25" state="hidden" r:id="rId17"/>
@@ -6921,57 +6921,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="68" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -7118,6 +7067,57 @@
     </xf>
     <xf numFmtId="0" fontId="69" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -9623,7 +9623,7 @@
   <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D196" sqref="D196"/>
+      <selection activeCell="L180" sqref="L180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12085,14 +12085,14 @@
       <c r="B4" t="s">
         <v>1148</v>
       </c>
-      <c r="C4" s="117" t="s">
+      <c r="C4" s="166" t="s">
         <v>1155</v>
       </c>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117" t="s">
+      <c r="D4" s="166"/>
+      <c r="E4" s="166" t="s">
         <v>1156</v>
       </c>
-      <c r="F4" s="117"/>
+      <c r="F4" s="166"/>
     </row>
     <row r="5" spans="2:10">
       <c r="C5" t="s">
@@ -12448,7 +12448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
@@ -13228,147 +13228,147 @@
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="154" t="s">
         <v>474</v>
       </c>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
     </row>
     <row r="2" spans="1:31">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="150" t="s">
         <v>475</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="102" t="s">
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="155" t="s">
         <v>476</v>
       </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="102" t="s">
+      <c r="F2" s="156"/>
+      <c r="G2" s="155" t="s">
         <v>477</v>
       </c>
-      <c r="H2" s="103"/>
+      <c r="H2" s="156"/>
     </row>
     <row r="3" spans="1:31">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="152" t="s">
         <v>478</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="101">
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="157">
         <v>1</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101">
+      <c r="F3" s="157"/>
+      <c r="G3" s="157">
         <v>1</v>
       </c>
-      <c r="H3" s="101"/>
+      <c r="H3" s="157"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="152" t="s">
         <v>479</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="101">
+      <c r="C4" s="153"/>
+      <c r="D4" s="153"/>
+      <c r="E4" s="157">
         <v>2</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101">
+      <c r="F4" s="157"/>
+      <c r="G4" s="157">
         <v>2</v>
       </c>
-      <c r="H4" s="101"/>
+      <c r="H4" s="157"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="152" t="s">
         <v>480</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="101">
+      <c r="C5" s="153"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="157">
         <v>4</v>
       </c>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101">
+      <c r="F5" s="157"/>
+      <c r="G5" s="157">
         <v>4</v>
       </c>
-      <c r="H5" s="101"/>
+      <c r="H5" s="157"/>
     </row>
     <row r="6" spans="1:31">
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="152" t="s">
         <v>481</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="106">
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="158">
         <v>8</v>
       </c>
-      <c r="F6" s="106"/>
-      <c r="G6" s="101">
+      <c r="F6" s="158"/>
+      <c r="G6" s="157">
         <v>4</v>
       </c>
-      <c r="H6" s="101"/>
+      <c r="H6" s="157"/>
     </row>
     <row r="7" spans="1:31">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="152" t="s">
         <v>482</v>
       </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="101">
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="157">
         <v>8</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101">
+      <c r="F7" s="157"/>
+      <c r="G7" s="157">
         <v>8</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="157"/>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="152" t="s">
         <v>483</v>
       </c>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="101">
+      <c r="C8" s="153"/>
+      <c r="D8" s="153"/>
+      <c r="E8" s="157">
         <v>4</v>
       </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101">
+      <c r="F8" s="157"/>
+      <c r="G8" s="157">
         <v>4</v>
       </c>
-      <c r="H8" s="101"/>
+      <c r="H8" s="157"/>
     </row>
     <row r="9" spans="1:31">
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="152" t="s">
         <v>484</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="101">
+      <c r="C9" s="153"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="157">
         <v>8</v>
       </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101">
+      <c r="F9" s="157"/>
+      <c r="G9" s="157">
         <v>8</v>
       </c>
-      <c r="H9" s="101"/>
+      <c r="H9" s="157"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="152" t="s">
         <v>485</v>
       </c>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="106">
+      <c r="C10" s="153"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="158">
         <v>8</v>
       </c>
-      <c r="F10" s="106"/>
-      <c r="G10" s="101">
+      <c r="F10" s="158"/>
+      <c r="G10" s="157">
         <v>4</v>
       </c>
-      <c r="H10" s="101"/>
+      <c r="H10" s="157"/>
     </row>
     <row r="13" spans="1:31" ht="15.75">
       <c r="A13" s="28" t="s">
@@ -13661,12 +13661,12 @@
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
-      <c r="H23" s="107" t="s">
+      <c r="H23" s="160" t="s">
         <v>474</v>
       </c>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="109"/>
+      <c r="I23" s="161"/>
+      <c r="J23" s="161"/>
+      <c r="K23" s="162"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
@@ -13689,510 +13689,561 @@
       <c r="AE23" s="26"/>
     </row>
     <row r="24" spans="1:33">
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="163" t="s">
         <v>475</v>
       </c>
-      <c r="C24" s="110"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="110"/>
-      <c r="G24" s="110"/>
-      <c r="H24" s="102" t="s">
+      <c r="C24" s="163"/>
+      <c r="D24" s="163"/>
+      <c r="E24" s="163"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="163"/>
+      <c r="H24" s="155" t="s">
         <v>476</v>
       </c>
-      <c r="I24" s="103"/>
-      <c r="J24" s="102" t="s">
+      <c r="I24" s="156"/>
+      <c r="J24" s="155" t="s">
         <v>477</v>
       </c>
-      <c r="K24" s="103"/>
-      <c r="L24" s="105" t="s">
+      <c r="K24" s="156"/>
+      <c r="L24" s="164" t="s">
         <v>495</v>
       </c>
-      <c r="M24" s="105"/>
-      <c r="N24" s="105"/>
-      <c r="O24" s="105"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="105"/>
-      <c r="R24" s="105"/>
-      <c r="S24" s="105"/>
-      <c r="T24" s="105"/>
-      <c r="U24" s="105"/>
-      <c r="V24" s="105"/>
-      <c r="W24" s="105"/>
-      <c r="X24" s="105"/>
-      <c r="Y24" s="105"/>
-      <c r="Z24" s="105"/>
-      <c r="AA24" s="105"/>
-      <c r="AB24" s="105"/>
-      <c r="AC24" s="105"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="105"/>
+      <c r="M24" s="164"/>
+      <c r="N24" s="164"/>
+      <c r="O24" s="164"/>
+      <c r="P24" s="164"/>
+      <c r="Q24" s="164"/>
+      <c r="R24" s="164"/>
+      <c r="S24" s="164"/>
+      <c r="T24" s="164"/>
+      <c r="U24" s="164"/>
+      <c r="V24" s="164"/>
+      <c r="W24" s="164"/>
+      <c r="X24" s="164"/>
+      <c r="Y24" s="164"/>
+      <c r="Z24" s="164"/>
+      <c r="AA24" s="164"/>
+      <c r="AB24" s="164"/>
+      <c r="AC24" s="164"/>
+      <c r="AD24" s="164"/>
+      <c r="AE24" s="164"/>
     </row>
     <row r="25" spans="1:33">
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="159" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="104"/>
-      <c r="H25" s="101">
+      <c r="C25" s="159"/>
+      <c r="D25" s="159"/>
+      <c r="E25" s="159"/>
+      <c r="F25" s="159"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="157">
         <v>1</v>
       </c>
-      <c r="I25" s="101"/>
-      <c r="J25" s="101">
+      <c r="I25" s="157"/>
+      <c r="J25" s="157">
         <v>1</v>
       </c>
-      <c r="K25" s="101"/>
-      <c r="L25" s="104" t="s">
+      <c r="K25" s="157"/>
+      <c r="L25" s="159" t="s">
         <v>497</v>
       </c>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="104"/>
-      <c r="Q25" s="104"/>
-      <c r="R25" s="104"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="104"/>
-      <c r="U25" s="104"/>
-      <c r="V25" s="104"/>
-      <c r="W25" s="104"/>
-      <c r="X25" s="104"/>
-      <c r="Y25" s="104"/>
-      <c r="Z25" s="104"/>
-      <c r="AA25" s="104"/>
-      <c r="AB25" s="104"/>
-      <c r="AC25" s="104"/>
-      <c r="AD25" s="104"/>
-      <c r="AE25" s="104"/>
+      <c r="M25" s="159"/>
+      <c r="N25" s="159"/>
+      <c r="O25" s="159"/>
+      <c r="P25" s="159"/>
+      <c r="Q25" s="159"/>
+      <c r="R25" s="159"/>
+      <c r="S25" s="159"/>
+      <c r="T25" s="159"/>
+      <c r="U25" s="159"/>
+      <c r="V25" s="159"/>
+      <c r="W25" s="159"/>
+      <c r="X25" s="159"/>
+      <c r="Y25" s="159"/>
+      <c r="Z25" s="159"/>
+      <c r="AA25" s="159"/>
+      <c r="AB25" s="159"/>
+      <c r="AC25" s="159"/>
+      <c r="AD25" s="159"/>
+      <c r="AE25" s="159"/>
     </row>
     <row r="26" spans="1:33">
-      <c r="B26" s="104" t="s">
+      <c r="B26" s="159" t="s">
         <v>498</v>
       </c>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="104"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="101">
+      <c r="C26" s="159"/>
+      <c r="D26" s="159"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="157">
         <v>2</v>
       </c>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101">
+      <c r="I26" s="157"/>
+      <c r="J26" s="157">
         <v>2</v>
       </c>
-      <c r="K26" s="101"/>
-      <c r="L26" s="104" t="s">
+      <c r="K26" s="157"/>
+      <c r="L26" s="159" t="s">
         <v>499</v>
       </c>
-      <c r="M26" s="104"/>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
-      <c r="S26" s="104"/>
-      <c r="T26" s="104"/>
-      <c r="U26" s="104"/>
-      <c r="V26" s="104"/>
-      <c r="W26" s="104"/>
-      <c r="X26" s="104"/>
-      <c r="Y26" s="104"/>
-      <c r="Z26" s="104"/>
-      <c r="AA26" s="104"/>
-      <c r="AB26" s="104"/>
-      <c r="AC26" s="104"/>
-      <c r="AD26" s="104"/>
-      <c r="AE26" s="104"/>
+      <c r="M26" s="159"/>
+      <c r="N26" s="159"/>
+      <c r="O26" s="159"/>
+      <c r="P26" s="159"/>
+      <c r="Q26" s="159"/>
+      <c r="R26" s="159"/>
+      <c r="S26" s="159"/>
+      <c r="T26" s="159"/>
+      <c r="U26" s="159"/>
+      <c r="V26" s="159"/>
+      <c r="W26" s="159"/>
+      <c r="X26" s="159"/>
+      <c r="Y26" s="159"/>
+      <c r="Z26" s="159"/>
+      <c r="AA26" s="159"/>
+      <c r="AB26" s="159"/>
+      <c r="AC26" s="159"/>
+      <c r="AD26" s="159"/>
+      <c r="AE26" s="159"/>
     </row>
     <row r="27" spans="1:33">
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="159" t="s">
         <v>500</v>
       </c>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="104"/>
-      <c r="G27" s="104"/>
-      <c r="H27" s="101">
+      <c r="C27" s="159"/>
+      <c r="D27" s="159"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="159"/>
+      <c r="G27" s="159"/>
+      <c r="H27" s="157">
         <v>4</v>
       </c>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101">
+      <c r="I27" s="157"/>
+      <c r="J27" s="157">
         <v>4</v>
       </c>
-      <c r="K27" s="101"/>
-      <c r="L27" s="104" t="s">
+      <c r="K27" s="157"/>
+      <c r="L27" s="159" t="s">
         <v>501</v>
       </c>
-      <c r="M27" s="104"/>
-      <c r="N27" s="104"/>
-      <c r="O27" s="104"/>
-      <c r="P27" s="104"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
-      <c r="T27" s="104"/>
-      <c r="U27" s="104"/>
-      <c r="V27" s="104"/>
-      <c r="W27" s="104"/>
-      <c r="X27" s="104"/>
-      <c r="Y27" s="104"/>
-      <c r="Z27" s="104"/>
-      <c r="AA27" s="104"/>
-      <c r="AB27" s="104"/>
-      <c r="AC27" s="104"/>
-      <c r="AD27" s="104"/>
-      <c r="AE27" s="104"/>
+      <c r="M27" s="159"/>
+      <c r="N27" s="159"/>
+      <c r="O27" s="159"/>
+      <c r="P27" s="159"/>
+      <c r="Q27" s="159"/>
+      <c r="R27" s="159"/>
+      <c r="S27" s="159"/>
+      <c r="T27" s="159"/>
+      <c r="U27" s="159"/>
+      <c r="V27" s="159"/>
+      <c r="W27" s="159"/>
+      <c r="X27" s="159"/>
+      <c r="Y27" s="159"/>
+      <c r="Z27" s="159"/>
+      <c r="AA27" s="159"/>
+      <c r="AB27" s="159"/>
+      <c r="AC27" s="159"/>
+      <c r="AD27" s="159"/>
+      <c r="AE27" s="159"/>
     </row>
     <row r="28" spans="1:33">
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="159" t="s">
         <v>502</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="104"/>
-      <c r="H28" s="101">
+      <c r="C28" s="159"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="157">
         <v>4</v>
       </c>
-      <c r="I28" s="101"/>
-      <c r="J28" s="101">
+      <c r="I28" s="157"/>
+      <c r="J28" s="157">
         <v>4</v>
       </c>
-      <c r="K28" s="101"/>
-      <c r="L28" s="104" t="s">
+      <c r="K28" s="157"/>
+      <c r="L28" s="159" t="s">
         <v>503</v>
       </c>
-      <c r="M28" s="104"/>
-      <c r="N28" s="104"/>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
-      <c r="T28" s="104"/>
-      <c r="U28" s="104"/>
-      <c r="V28" s="104"/>
-      <c r="W28" s="104"/>
-      <c r="X28" s="104"/>
-      <c r="Y28" s="104"/>
-      <c r="Z28" s="104"/>
-      <c r="AA28" s="104"/>
-      <c r="AB28" s="104"/>
-      <c r="AC28" s="104"/>
-      <c r="AD28" s="104"/>
-      <c r="AE28" s="104"/>
+      <c r="M28" s="159"/>
+      <c r="N28" s="159"/>
+      <c r="O28" s="159"/>
+      <c r="P28" s="159"/>
+      <c r="Q28" s="159"/>
+      <c r="R28" s="159"/>
+      <c r="S28" s="159"/>
+      <c r="T28" s="159"/>
+      <c r="U28" s="159"/>
+      <c r="V28" s="159"/>
+      <c r="W28" s="159"/>
+      <c r="X28" s="159"/>
+      <c r="Y28" s="159"/>
+      <c r="Z28" s="159"/>
+      <c r="AA28" s="159"/>
+      <c r="AB28" s="159"/>
+      <c r="AC28" s="159"/>
+      <c r="AD28" s="159"/>
+      <c r="AE28" s="159"/>
     </row>
     <row r="29" spans="1:33">
-      <c r="B29" s="104" t="s">
+      <c r="B29" s="159" t="s">
         <v>504</v>
       </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="104"/>
-      <c r="H29" s="101">
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="157">
         <v>8</v>
       </c>
-      <c r="I29" s="101"/>
-      <c r="J29" s="101">
+      <c r="I29" s="157"/>
+      <c r="J29" s="157">
         <v>8</v>
       </c>
-      <c r="K29" s="101"/>
-      <c r="L29" s="104" t="s">
+      <c r="K29" s="157"/>
+      <c r="L29" s="159" t="s">
         <v>505</v>
       </c>
-      <c r="M29" s="104"/>
-      <c r="N29" s="104"/>
-      <c r="O29" s="104"/>
-      <c r="P29" s="104"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="104"/>
-      <c r="S29" s="104"/>
-      <c r="T29" s="104"/>
-      <c r="U29" s="104"/>
-      <c r="V29" s="104"/>
-      <c r="W29" s="104"/>
-      <c r="X29" s="104"/>
-      <c r="Y29" s="104"/>
-      <c r="Z29" s="104"/>
-      <c r="AA29" s="104"/>
-      <c r="AB29" s="104"/>
-      <c r="AC29" s="104"/>
-      <c r="AD29" s="104"/>
-      <c r="AE29" s="104"/>
+      <c r="M29" s="159"/>
+      <c r="N29" s="159"/>
+      <c r="O29" s="159"/>
+      <c r="P29" s="159"/>
+      <c r="Q29" s="159"/>
+      <c r="R29" s="159"/>
+      <c r="S29" s="159"/>
+      <c r="T29" s="159"/>
+      <c r="U29" s="159"/>
+      <c r="V29" s="159"/>
+      <c r="W29" s="159"/>
+      <c r="X29" s="159"/>
+      <c r="Y29" s="159"/>
+      <c r="Z29" s="159"/>
+      <c r="AA29" s="159"/>
+      <c r="AB29" s="159"/>
+      <c r="AC29" s="159"/>
+      <c r="AD29" s="159"/>
+      <c r="AE29" s="159"/>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="26"/>
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="159" t="s">
         <v>506</v>
       </c>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="106">
+      <c r="C30" s="159"/>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="158">
         <v>8</v>
       </c>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106">
+      <c r="I30" s="158"/>
+      <c r="J30" s="158">
         <v>4</v>
       </c>
-      <c r="K30" s="106"/>
-      <c r="L30" s="104" t="s">
+      <c r="K30" s="158"/>
+      <c r="L30" s="159" t="s">
         <v>507</v>
       </c>
-      <c r="M30" s="104"/>
-      <c r="N30" s="104"/>
-      <c r="O30" s="104"/>
-      <c r="P30" s="104"/>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="104"/>
-      <c r="S30" s="104"/>
-      <c r="T30" s="104"/>
-      <c r="U30" s="104"/>
-      <c r="V30" s="104"/>
-      <c r="W30" s="104"/>
-      <c r="X30" s="104"/>
-      <c r="Y30" s="104"/>
-      <c r="Z30" s="104"/>
-      <c r="AA30" s="104"/>
-      <c r="AB30" s="104"/>
-      <c r="AC30" s="104"/>
-      <c r="AD30" s="104"/>
-      <c r="AE30" s="104"/>
+      <c r="M30" s="159"/>
+      <c r="N30" s="159"/>
+      <c r="O30" s="159"/>
+      <c r="P30" s="159"/>
+      <c r="Q30" s="159"/>
+      <c r="R30" s="159"/>
+      <c r="S30" s="159"/>
+      <c r="T30" s="159"/>
+      <c r="U30" s="159"/>
+      <c r="V30" s="159"/>
+      <c r="W30" s="159"/>
+      <c r="X30" s="159"/>
+      <c r="Y30" s="159"/>
+      <c r="Z30" s="159"/>
+      <c r="AA30" s="159"/>
+      <c r="AB30" s="159"/>
+      <c r="AC30" s="159"/>
+      <c r="AD30" s="159"/>
+      <c r="AE30" s="159"/>
       <c r="AF30" s="26"/>
       <c r="AG30" s="26"/>
     </row>
     <row r="31" spans="1:33">
       <c r="A31" s="26"/>
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="159" t="s">
         <v>508</v>
       </c>
-      <c r="C31" s="104"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="104"/>
-      <c r="F31" s="104"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="106">
+      <c r="C31" s="159"/>
+      <c r="D31" s="159"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="158">
         <v>8</v>
       </c>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106">
+      <c r="I31" s="158"/>
+      <c r="J31" s="158">
         <v>4</v>
       </c>
-      <c r="K31" s="106"/>
-      <c r="L31" s="104" t="s">
+      <c r="K31" s="158"/>
+      <c r="L31" s="159" t="s">
         <v>509</v>
       </c>
-      <c r="M31" s="104"/>
-      <c r="N31" s="104"/>
-      <c r="O31" s="104"/>
-      <c r="P31" s="104"/>
-      <c r="Q31" s="104"/>
-      <c r="R31" s="104"/>
-      <c r="S31" s="104"/>
-      <c r="T31" s="104"/>
-      <c r="U31" s="104"/>
-      <c r="V31" s="104"/>
-      <c r="W31" s="104"/>
-      <c r="X31" s="104"/>
-      <c r="Y31" s="104"/>
-      <c r="Z31" s="104"/>
-      <c r="AA31" s="104"/>
-      <c r="AB31" s="104"/>
-      <c r="AC31" s="104"/>
-      <c r="AD31" s="104"/>
-      <c r="AE31" s="104"/>
+      <c r="M31" s="159"/>
+      <c r="N31" s="159"/>
+      <c r="O31" s="159"/>
+      <c r="P31" s="159"/>
+      <c r="Q31" s="159"/>
+      <c r="R31" s="159"/>
+      <c r="S31" s="159"/>
+      <c r="T31" s="159"/>
+      <c r="U31" s="159"/>
+      <c r="V31" s="159"/>
+      <c r="W31" s="159"/>
+      <c r="X31" s="159"/>
+      <c r="Y31" s="159"/>
+      <c r="Z31" s="159"/>
+      <c r="AA31" s="159"/>
+      <c r="AB31" s="159"/>
+      <c r="AC31" s="159"/>
+      <c r="AD31" s="159"/>
+      <c r="AE31" s="159"/>
       <c r="AF31" s="26"/>
       <c r="AG31" s="26"/>
     </row>
     <row r="32" spans="1:33">
       <c r="A32" s="26"/>
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="159" t="s">
         <v>483</v>
       </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="104"/>
-      <c r="F32" s="104"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="101">
+      <c r="C32" s="159"/>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="157">
         <v>4</v>
       </c>
-      <c r="I32" s="101"/>
-      <c r="J32" s="101">
+      <c r="I32" s="157"/>
+      <c r="J32" s="157">
         <v>4</v>
       </c>
-      <c r="K32" s="101"/>
-      <c r="L32" s="104" t="s">
+      <c r="K32" s="157"/>
+      <c r="L32" s="159" t="s">
         <v>510</v>
       </c>
-      <c r="M32" s="104"/>
-      <c r="N32" s="104"/>
-      <c r="O32" s="104"/>
-      <c r="P32" s="104"/>
-      <c r="Q32" s="104"/>
-      <c r="R32" s="104"/>
-      <c r="S32" s="104"/>
-      <c r="T32" s="104"/>
-      <c r="U32" s="104"/>
-      <c r="V32" s="104"/>
-      <c r="W32" s="104"/>
-      <c r="X32" s="104"/>
-      <c r="Y32" s="104"/>
-      <c r="Z32" s="104"/>
-      <c r="AA32" s="104"/>
-      <c r="AB32" s="104"/>
-      <c r="AC32" s="104"/>
-      <c r="AD32" s="104"/>
-      <c r="AE32" s="104"/>
+      <c r="M32" s="159"/>
+      <c r="N32" s="159"/>
+      <c r="O32" s="159"/>
+      <c r="P32" s="159"/>
+      <c r="Q32" s="159"/>
+      <c r="R32" s="159"/>
+      <c r="S32" s="159"/>
+      <c r="T32" s="159"/>
+      <c r="U32" s="159"/>
+      <c r="V32" s="159"/>
+      <c r="W32" s="159"/>
+      <c r="X32" s="159"/>
+      <c r="Y32" s="159"/>
+      <c r="Z32" s="159"/>
+      <c r="AA32" s="159"/>
+      <c r="AB32" s="159"/>
+      <c r="AC32" s="159"/>
+      <c r="AD32" s="159"/>
+      <c r="AE32" s="159"/>
       <c r="AF32" s="26"/>
       <c r="AG32" s="26"/>
     </row>
     <row r="33" spans="1:33">
       <c r="A33" s="26"/>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="159" t="s">
         <v>484</v>
       </c>
-      <c r="C33" s="104"/>
-      <c r="D33" s="104"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="104"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="101">
+      <c r="C33" s="159"/>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="159"/>
+      <c r="H33" s="157">
         <v>8</v>
       </c>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101">
+      <c r="I33" s="157"/>
+      <c r="J33" s="157">
         <v>8</v>
       </c>
-      <c r="K33" s="101"/>
-      <c r="L33" s="104" t="s">
+      <c r="K33" s="157"/>
+      <c r="L33" s="159" t="s">
         <v>511</v>
       </c>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="104"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="104"/>
-      <c r="S33" s="104"/>
-      <c r="T33" s="104"/>
-      <c r="U33" s="104"/>
-      <c r="V33" s="104"/>
-      <c r="W33" s="104"/>
-      <c r="X33" s="104"/>
-      <c r="Y33" s="104"/>
-      <c r="Z33" s="104"/>
-      <c r="AA33" s="104"/>
-      <c r="AB33" s="104"/>
-      <c r="AC33" s="104"/>
-      <c r="AD33" s="104"/>
-      <c r="AE33" s="104"/>
+      <c r="M33" s="159"/>
+      <c r="N33" s="159"/>
+      <c r="O33" s="159"/>
+      <c r="P33" s="159"/>
+      <c r="Q33" s="159"/>
+      <c r="R33" s="159"/>
+      <c r="S33" s="159"/>
+      <c r="T33" s="159"/>
+      <c r="U33" s="159"/>
+      <c r="V33" s="159"/>
+      <c r="W33" s="159"/>
+      <c r="X33" s="159"/>
+      <c r="Y33" s="159"/>
+      <c r="Z33" s="159"/>
+      <c r="AA33" s="159"/>
+      <c r="AB33" s="159"/>
+      <c r="AC33" s="159"/>
+      <c r="AD33" s="159"/>
+      <c r="AE33" s="159"/>
       <c r="AF33" s="26"/>
       <c r="AG33" s="26"/>
     </row>
     <row r="34" spans="1:33">
       <c r="A34" s="26"/>
-      <c r="B34" s="104" t="s">
+      <c r="B34" s="159" t="s">
         <v>512</v>
       </c>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="104"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="101">
+      <c r="C34" s="159"/>
+      <c r="D34" s="159"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="157">
         <v>8</v>
       </c>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101">
+      <c r="I34" s="157"/>
+      <c r="J34" s="157">
         <v>8</v>
       </c>
-      <c r="K34" s="101"/>
-      <c r="L34" s="104" t="s">
+      <c r="K34" s="157"/>
+      <c r="L34" s="159" t="s">
         <v>505</v>
       </c>
-      <c r="M34" s="104"/>
-      <c r="N34" s="104"/>
-      <c r="O34" s="104"/>
-      <c r="P34" s="104"/>
-      <c r="Q34" s="104"/>
-      <c r="R34" s="104"/>
-      <c r="S34" s="104"/>
-      <c r="T34" s="104"/>
-      <c r="U34" s="104"/>
-      <c r="V34" s="104"/>
-      <c r="W34" s="104"/>
-      <c r="X34" s="104"/>
-      <c r="Y34" s="104"/>
-      <c r="Z34" s="104"/>
-      <c r="AA34" s="104"/>
-      <c r="AB34" s="104"/>
-      <c r="AC34" s="104"/>
-      <c r="AD34" s="104"/>
-      <c r="AE34" s="104"/>
+      <c r="M34" s="159"/>
+      <c r="N34" s="159"/>
+      <c r="O34" s="159"/>
+      <c r="P34" s="159"/>
+      <c r="Q34" s="159"/>
+      <c r="R34" s="159"/>
+      <c r="S34" s="159"/>
+      <c r="T34" s="159"/>
+      <c r="U34" s="159"/>
+      <c r="V34" s="159"/>
+      <c r="W34" s="159"/>
+      <c r="X34" s="159"/>
+      <c r="Y34" s="159"/>
+      <c r="Z34" s="159"/>
+      <c r="AA34" s="159"/>
+      <c r="AB34" s="159"/>
+      <c r="AC34" s="159"/>
+      <c r="AD34" s="159"/>
+      <c r="AE34" s="159"/>
       <c r="AF34" s="26"/>
       <c r="AG34" s="26"/>
     </row>
     <row r="35" spans="1:33">
       <c r="A35" s="26"/>
-      <c r="B35" s="104" t="s">
+      <c r="B35" s="159" t="s">
         <v>513</v>
       </c>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="106">
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="159"/>
+      <c r="H35" s="158">
         <v>8</v>
       </c>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106">
+      <c r="I35" s="158"/>
+      <c r="J35" s="158">
         <v>4</v>
       </c>
-      <c r="K35" s="106"/>
-      <c r="L35" s="104" t="s">
+      <c r="K35" s="158"/>
+      <c r="L35" s="159" t="s">
         <v>514</v>
       </c>
-      <c r="M35" s="104"/>
-      <c r="N35" s="104"/>
-      <c r="O35" s="104"/>
-      <c r="P35" s="104"/>
-      <c r="Q35" s="104"/>
-      <c r="R35" s="104"/>
-      <c r="S35" s="104"/>
-      <c r="T35" s="104"/>
-      <c r="U35" s="104"/>
-      <c r="V35" s="104"/>
-      <c r="W35" s="104"/>
-      <c r="X35" s="104"/>
-      <c r="Y35" s="104"/>
-      <c r="Z35" s="104"/>
-      <c r="AA35" s="104"/>
-      <c r="AB35" s="104"/>
-      <c r="AC35" s="104"/>
-      <c r="AD35" s="104"/>
-      <c r="AE35" s="104"/>
+      <c r="M35" s="159"/>
+      <c r="N35" s="159"/>
+      <c r="O35" s="159"/>
+      <c r="P35" s="159"/>
+      <c r="Q35" s="159"/>
+      <c r="R35" s="159"/>
+      <c r="S35" s="159"/>
+      <c r="T35" s="159"/>
+      <c r="U35" s="159"/>
+      <c r="V35" s="159"/>
+      <c r="W35" s="159"/>
+      <c r="X35" s="159"/>
+      <c r="Y35" s="159"/>
+      <c r="Z35" s="159"/>
+      <c r="AA35" s="159"/>
+      <c r="AB35" s="159"/>
+      <c r="AC35" s="159"/>
+      <c r="AD35" s="159"/>
+      <c r="AE35" s="159"/>
       <c r="AF35" s="26"/>
       <c r="AG35" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L25:AE25"/>
+    <mergeCell ref="L24:AE24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L35:AE35"/>
+    <mergeCell ref="L27:AE27"/>
+    <mergeCell ref="L26:AE26"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="L31:AE31"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="L30:AE30"/>
+    <mergeCell ref="L32:AE32"/>
+    <mergeCell ref="L28:AE28"/>
+    <mergeCell ref="L33:AE33"/>
+    <mergeCell ref="L34:AE34"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="L29:AE29"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B4:D4"/>
@@ -14209,62 +14260,11 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="L31:AE31"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="L30:AE30"/>
-    <mergeCell ref="L32:AE32"/>
-    <mergeCell ref="L28:AE28"/>
-    <mergeCell ref="L33:AE33"/>
-    <mergeCell ref="L34:AE34"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="L29:AE29"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L35:AE35"/>
-    <mergeCell ref="L27:AE27"/>
-    <mergeCell ref="L26:AE26"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L25:AE25"/>
-    <mergeCell ref="L24:AE24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14831,1537 +14831,1537 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BR53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="119" customWidth="1"/>
-    <col min="2" max="3" width="2.5703125" style="119"/>
-    <col min="4" max="4" width="5.28515625" style="119" customWidth="1"/>
-    <col min="5" max="5" width="2.5703125" style="119" customWidth="1"/>
-    <col min="6" max="9" width="2.5703125" style="119"/>
-    <col min="10" max="10" width="2.5703125" style="119" customWidth="1"/>
-    <col min="11" max="16384" width="2.5703125" style="119"/>
+    <col min="1" max="1" width="2.7109375" style="102" customWidth="1"/>
+    <col min="2" max="3" width="2.5703125" style="102"/>
+    <col min="4" max="4" width="5.28515625" style="102" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" style="102" customWidth="1"/>
+    <col min="6" max="9" width="2.5703125" style="102"/>
+    <col min="10" max="10" width="2.5703125" style="102" customWidth="1"/>
+    <col min="11" max="16384" width="2.5703125" style="102"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:52">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="101" t="s">
         <v>1356</v>
       </c>
     </row>
     <row r="4" spans="1:52">
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="103" t="s">
         <v>1357</v>
       </c>
     </row>
     <row r="6" spans="1:52">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="104" t="s">
         <v>1358</v>
       </c>
     </row>
     <row r="7" spans="1:52" ht="15" thickBot="1">
-      <c r="B7" s="122"/>
-      <c r="C7" s="123" t="s">
+      <c r="B7" s="105"/>
+      <c r="C7" s="106" t="s">
         <v>1359</v>
       </c>
-      <c r="D7" s="124"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="123" t="s">
+      <c r="D7" s="107"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="106" t="s">
         <v>1360</v>
       </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-      <c r="Q7" s="124"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="124"/>
-      <c r="T7" s="124"/>
-      <c r="U7" s="124"/>
-      <c r="V7" s="124"/>
-      <c r="W7" s="124"/>
-      <c r="X7" s="124"/>
-      <c r="Y7" s="124"/>
-      <c r="Z7" s="124"/>
-      <c r="AA7" s="124"/>
-      <c r="AB7" s="124"/>
-      <c r="AC7" s="124"/>
-      <c r="AD7" s="124"/>
-      <c r="AE7" s="124"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="124"/>
-      <c r="AH7" s="124"/>
-      <c r="AI7" s="124"/>
-      <c r="AJ7" s="124"/>
-      <c r="AK7" s="124"/>
-      <c r="AL7" s="124"/>
-      <c r="AM7" s="124"/>
-      <c r="AN7" s="124"/>
-      <c r="AO7" s="124"/>
-      <c r="AP7" s="124"/>
-      <c r="AQ7" s="124"/>
-      <c r="AR7" s="124"/>
-      <c r="AS7" s="124"/>
-      <c r="AT7" s="124"/>
-      <c r="AU7" s="124"/>
-      <c r="AV7" s="124"/>
-      <c r="AW7" s="125"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="107"/>
+      <c r="AB7" s="107"/>
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
+      <c r="AE7" s="107"/>
+      <c r="AF7" s="107"/>
+      <c r="AG7" s="107"/>
+      <c r="AH7" s="107"/>
+      <c r="AI7" s="107"/>
+      <c r="AJ7" s="107"/>
+      <c r="AK7" s="107"/>
+      <c r="AL7" s="107"/>
+      <c r="AM7" s="107"/>
+      <c r="AN7" s="107"/>
+      <c r="AO7" s="107"/>
+      <c r="AP7" s="107"/>
+      <c r="AQ7" s="107"/>
+      <c r="AR7" s="107"/>
+      <c r="AS7" s="107"/>
+      <c r="AT7" s="107"/>
+      <c r="AU7" s="107"/>
+      <c r="AV7" s="107"/>
+      <c r="AW7" s="108"/>
     </row>
     <row r="8" spans="1:52" ht="15" thickTop="1">
-      <c r="C8" s="126" t="s">
+      <c r="C8" s="109" t="s">
         <v>1361</v>
       </c>
-      <c r="D8" s="127"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="129" t="s">
+      <c r="D8" s="110"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="112" t="s">
         <v>1362</v>
       </c>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="127"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="127"/>
-      <c r="P8" s="127"/>
-      <c r="Q8" s="127"/>
-      <c r="R8" s="127"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="127"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="127"/>
-      <c r="Y8" s="127"/>
-      <c r="Z8" s="127"/>
-      <c r="AA8" s="127"/>
-      <c r="AB8" s="127"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="127"/>
-      <c r="AE8" s="127"/>
-      <c r="AF8" s="127"/>
-      <c r="AG8" s="127"/>
-      <c r="AH8" s="127"/>
-      <c r="AI8" s="127"/>
-      <c r="AJ8" s="127"/>
-      <c r="AK8" s="127"/>
-      <c r="AL8" s="127"/>
-      <c r="AM8" s="127"/>
-      <c r="AN8" s="127"/>
-      <c r="AO8" s="127"/>
-      <c r="AP8" s="127"/>
-      <c r="AQ8" s="127"/>
-      <c r="AR8" s="127"/>
-      <c r="AS8" s="127"/>
-      <c r="AT8" s="127"/>
-      <c r="AU8" s="127"/>
-      <c r="AV8" s="127"/>
-      <c r="AW8" s="128"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="110"/>
+      <c r="K8" s="110"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="110"/>
+      <c r="N8" s="110"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="110"/>
+      <c r="W8" s="110"/>
+      <c r="X8" s="110"/>
+      <c r="Y8" s="110"/>
+      <c r="Z8" s="110"/>
+      <c r="AA8" s="110"/>
+      <c r="AB8" s="110"/>
+      <c r="AC8" s="110"/>
+      <c r="AD8" s="110"/>
+      <c r="AE8" s="110"/>
+      <c r="AF8" s="110"/>
+      <c r="AG8" s="110"/>
+      <c r="AH8" s="110"/>
+      <c r="AI8" s="110"/>
+      <c r="AJ8" s="110"/>
+      <c r="AK8" s="110"/>
+      <c r="AL8" s="110"/>
+      <c r="AM8" s="110"/>
+      <c r="AN8" s="110"/>
+      <c r="AO8" s="110"/>
+      <c r="AP8" s="110"/>
+      <c r="AQ8" s="110"/>
+      <c r="AR8" s="110"/>
+      <c r="AS8" s="110"/>
+      <c r="AT8" s="110"/>
+      <c r="AU8" s="110"/>
+      <c r="AV8" s="110"/>
+      <c r="AW8" s="111"/>
     </row>
     <row r="9" spans="1:52">
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="113" t="s">
         <v>1363</v>
       </c>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="133" t="s">
+      <c r="D9" s="114"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="116" t="s">
         <v>1364</v>
       </c>
-      <c r="G9" s="131"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="131"/>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="131"/>
-      <c r="N9" s="131"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="131"/>
-      <c r="R9" s="131"/>
-      <c r="S9" s="131"/>
-      <c r="T9" s="131"/>
-      <c r="U9" s="131"/>
-      <c r="V9" s="131"/>
-      <c r="W9" s="131"/>
-      <c r="X9" s="131"/>
-      <c r="Y9" s="131"/>
-      <c r="Z9" s="131"/>
-      <c r="AA9" s="131"/>
-      <c r="AB9" s="131"/>
-      <c r="AC9" s="131"/>
-      <c r="AD9" s="131"/>
-      <c r="AE9" s="131"/>
-      <c r="AF9" s="131"/>
-      <c r="AG9" s="131"/>
-      <c r="AH9" s="131"/>
-      <c r="AI9" s="131"/>
-      <c r="AJ9" s="131"/>
-      <c r="AK9" s="131"/>
-      <c r="AL9" s="131"/>
-      <c r="AM9" s="131"/>
-      <c r="AN9" s="131"/>
-      <c r="AO9" s="131"/>
-      <c r="AP9" s="131"/>
-      <c r="AQ9" s="131"/>
-      <c r="AR9" s="131"/>
-      <c r="AS9" s="131"/>
-      <c r="AT9" s="131"/>
-      <c r="AU9" s="131"/>
-      <c r="AV9" s="131"/>
-      <c r="AW9" s="132"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114"/>
+      <c r="R9" s="114"/>
+      <c r="S9" s="114"/>
+      <c r="T9" s="114"/>
+      <c r="U9" s="114"/>
+      <c r="V9" s="114"/>
+      <c r="W9" s="114"/>
+      <c r="X9" s="114"/>
+      <c r="Y9" s="114"/>
+      <c r="Z9" s="114"/>
+      <c r="AA9" s="114"/>
+      <c r="AB9" s="114"/>
+      <c r="AC9" s="114"/>
+      <c r="AD9" s="114"/>
+      <c r="AE9" s="114"/>
+      <c r="AF9" s="114"/>
+      <c r="AG9" s="114"/>
+      <c r="AH9" s="114"/>
+      <c r="AI9" s="114"/>
+      <c r="AJ9" s="114"/>
+      <c r="AK9" s="114"/>
+      <c r="AL9" s="114"/>
+      <c r="AM9" s="114"/>
+      <c r="AN9" s="114"/>
+      <c r="AO9" s="114"/>
+      <c r="AP9" s="114"/>
+      <c r="AQ9" s="114"/>
+      <c r="AR9" s="114"/>
+      <c r="AS9" s="114"/>
+      <c r="AT9" s="114"/>
+      <c r="AU9" s="114"/>
+      <c r="AV9" s="114"/>
+      <c r="AW9" s="115"/>
     </row>
     <row r="10" spans="1:52">
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="117" t="s">
         <v>1365</v>
       </c>
-      <c r="D10" s="135"/>
-      <c r="E10" s="136"/>
-      <c r="F10" s="137" t="s">
+      <c r="D10" s="118"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="120" t="s">
         <v>1366</v>
       </c>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="135"/>
-      <c r="L10" s="135"/>
-      <c r="M10" s="135"/>
-      <c r="N10" s="135"/>
-      <c r="O10" s="135"/>
-      <c r="P10" s="135"/>
-      <c r="Q10" s="135"/>
-      <c r="R10" s="135"/>
-      <c r="S10" s="135"/>
-      <c r="T10" s="135"/>
-      <c r="U10" s="135"/>
-      <c r="V10" s="135"/>
-      <c r="W10" s="135"/>
-      <c r="X10" s="135"/>
-      <c r="Y10" s="135"/>
-      <c r="Z10" s="135"/>
-      <c r="AA10" s="135"/>
-      <c r="AB10" s="135"/>
-      <c r="AC10" s="135"/>
-      <c r="AD10" s="135"/>
-      <c r="AE10" s="135"/>
-      <c r="AF10" s="135"/>
-      <c r="AG10" s="135"/>
-      <c r="AH10" s="135"/>
-      <c r="AI10" s="135"/>
-      <c r="AJ10" s="135"/>
-      <c r="AK10" s="135"/>
-      <c r="AL10" s="135"/>
-      <c r="AM10" s="135"/>
-      <c r="AN10" s="135"/>
-      <c r="AO10" s="135"/>
-      <c r="AP10" s="135"/>
-      <c r="AQ10" s="135"/>
-      <c r="AR10" s="135"/>
-      <c r="AS10" s="135"/>
-      <c r="AT10" s="135"/>
-      <c r="AU10" s="135"/>
-      <c r="AV10" s="135"/>
-      <c r="AW10" s="136"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+      <c r="O10" s="118"/>
+      <c r="P10" s="118"/>
+      <c r="Q10" s="118"/>
+      <c r="R10" s="118"/>
+      <c r="S10" s="118"/>
+      <c r="T10" s="118"/>
+      <c r="U10" s="118"/>
+      <c r="V10" s="118"/>
+      <c r="W10" s="118"/>
+      <c r="X10" s="118"/>
+      <c r="Y10" s="118"/>
+      <c r="Z10" s="118"/>
+      <c r="AA10" s="118"/>
+      <c r="AB10" s="118"/>
+      <c r="AC10" s="118"/>
+      <c r="AD10" s="118"/>
+      <c r="AE10" s="118"/>
+      <c r="AF10" s="118"/>
+      <c r="AG10" s="118"/>
+      <c r="AH10" s="118"/>
+      <c r="AI10" s="118"/>
+      <c r="AJ10" s="118"/>
+      <c r="AK10" s="118"/>
+      <c r="AL10" s="118"/>
+      <c r="AM10" s="118"/>
+      <c r="AN10" s="118"/>
+      <c r="AO10" s="118"/>
+      <c r="AP10" s="118"/>
+      <c r="AQ10" s="118"/>
+      <c r="AR10" s="118"/>
+      <c r="AS10" s="118"/>
+      <c r="AT10" s="118"/>
+      <c r="AU10" s="118"/>
+      <c r="AV10" s="118"/>
+      <c r="AW10" s="119"/>
     </row>
     <row r="12" spans="1:52">
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="104" t="s">
         <v>1367</v>
       </c>
     </row>
     <row r="13" spans="1:52">
-      <c r="C13" s="138" t="s">
+      <c r="C13" s="121" t="s">
         <v>1368</v>
       </c>
     </row>
     <row r="15" spans="1:52" ht="15" thickBot="1">
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="122" t="s">
         <v>1369</v>
       </c>
-      <c r="D15" s="124"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="123" t="s">
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="106" t="s">
         <v>1360</v>
       </c>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
-      <c r="Q15" s="124"/>
-      <c r="R15" s="124"/>
-      <c r="S15" s="124"/>
-      <c r="T15" s="124"/>
-      <c r="U15" s="124"/>
-      <c r="V15" s="124"/>
-      <c r="W15" s="124"/>
-      <c r="X15" s="124"/>
-      <c r="Y15" s="124"/>
-      <c r="Z15" s="124"/>
-      <c r="AA15" s="124"/>
-      <c r="AB15" s="124"/>
-      <c r="AC15" s="124"/>
-      <c r="AD15" s="125"/>
-      <c r="AE15" s="140" t="s">
+      <c r="J15" s="107"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="107"/>
+      <c r="O15" s="107"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
+      <c r="U15" s="107"/>
+      <c r="V15" s="107"/>
+      <c r="W15" s="107"/>
+      <c r="X15" s="107"/>
+      <c r="Y15" s="107"/>
+      <c r="Z15" s="107"/>
+      <c r="AA15" s="107"/>
+      <c r="AB15" s="107"/>
+      <c r="AC15" s="107"/>
+      <c r="AD15" s="108"/>
+      <c r="AE15" s="123" t="s">
         <v>1370</v>
       </c>
-      <c r="AF15" s="124"/>
-      <c r="AG15" s="124"/>
-      <c r="AH15" s="124"/>
-      <c r="AI15" s="124"/>
-      <c r="AJ15" s="124"/>
-      <c r="AK15" s="124"/>
-      <c r="AL15" s="124"/>
-      <c r="AM15" s="124"/>
-      <c r="AN15" s="124"/>
-      <c r="AO15" s="124"/>
-      <c r="AP15" s="124"/>
-      <c r="AQ15" s="124"/>
-      <c r="AR15" s="124"/>
-      <c r="AS15" s="124"/>
-      <c r="AT15" s="124"/>
-      <c r="AU15" s="124"/>
-      <c r="AV15" s="124"/>
-      <c r="AW15" s="124"/>
-      <c r="AX15" s="124"/>
-      <c r="AY15" s="124"/>
-      <c r="AZ15" s="125"/>
+      <c r="AF15" s="107"/>
+      <c r="AG15" s="107"/>
+      <c r="AH15" s="107"/>
+      <c r="AI15" s="107"/>
+      <c r="AJ15" s="107"/>
+      <c r="AK15" s="107"/>
+      <c r="AL15" s="107"/>
+      <c r="AM15" s="107"/>
+      <c r="AN15" s="107"/>
+      <c r="AO15" s="107"/>
+      <c r="AP15" s="107"/>
+      <c r="AQ15" s="107"/>
+      <c r="AR15" s="107"/>
+      <c r="AS15" s="107"/>
+      <c r="AT15" s="107"/>
+      <c r="AU15" s="107"/>
+      <c r="AV15" s="107"/>
+      <c r="AW15" s="107"/>
+      <c r="AX15" s="107"/>
+      <c r="AY15" s="107"/>
+      <c r="AZ15" s="108"/>
     </row>
     <row r="16" spans="1:52" ht="15" thickTop="1">
-      <c r="A16" s="141"/>
-      <c r="C16" s="126" t="s">
+      <c r="A16" s="124"/>
+      <c r="C16" s="109" t="s">
         <v>1371</v>
       </c>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="127"/>
-      <c r="G16" s="127"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="120" t="s">
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="103" t="s">
         <v>1372</v>
       </c>
-      <c r="J16" s="127"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="127"/>
-      <c r="M16" s="127"/>
-      <c r="N16" s="127"/>
-      <c r="O16" s="127"/>
-      <c r="P16" s="127"/>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="127"/>
-      <c r="S16" s="127"/>
-      <c r="T16" s="127"/>
-      <c r="U16" s="127"/>
-      <c r="V16" s="127"/>
-      <c r="W16" s="127"/>
-      <c r="X16" s="127"/>
-      <c r="Y16" s="127"/>
-      <c r="Z16" s="127"/>
-      <c r="AA16" s="127"/>
-      <c r="AB16" s="127"/>
-      <c r="AC16" s="127"/>
-      <c r="AD16" s="128"/>
-      <c r="AE16" s="142" t="s">
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
+      <c r="N16" s="110"/>
+      <c r="O16" s="110"/>
+      <c r="P16" s="110"/>
+      <c r="Q16" s="110"/>
+      <c r="R16" s="110"/>
+      <c r="S16" s="110"/>
+      <c r="T16" s="110"/>
+      <c r="U16" s="110"/>
+      <c r="V16" s="110"/>
+      <c r="W16" s="110"/>
+      <c r="X16" s="110"/>
+      <c r="Y16" s="110"/>
+      <c r="Z16" s="110"/>
+      <c r="AA16" s="110"/>
+      <c r="AB16" s="110"/>
+      <c r="AC16" s="110"/>
+      <c r="AD16" s="111"/>
+      <c r="AE16" s="125" t="s">
         <v>1373</v>
       </c>
-      <c r="AF16" s="127"/>
-      <c r="AG16" s="127"/>
-      <c r="AH16" s="127"/>
-      <c r="AI16" s="127"/>
-      <c r="AJ16" s="127"/>
-      <c r="AK16" s="127"/>
-      <c r="AL16" s="127"/>
-      <c r="AM16" s="127"/>
-      <c r="AN16" s="127"/>
-      <c r="AO16" s="127"/>
-      <c r="AP16" s="127"/>
-      <c r="AQ16" s="127"/>
-      <c r="AR16" s="127"/>
-      <c r="AS16" s="127"/>
-      <c r="AT16" s="127"/>
-      <c r="AU16" s="127"/>
-      <c r="AV16" s="127"/>
-      <c r="AW16" s="127"/>
-      <c r="AX16" s="127"/>
-      <c r="AY16" s="127"/>
-      <c r="AZ16" s="128"/>
+      <c r="AF16" s="110"/>
+      <c r="AG16" s="110"/>
+      <c r="AH16" s="110"/>
+      <c r="AI16" s="110"/>
+      <c r="AJ16" s="110"/>
+      <c r="AK16" s="110"/>
+      <c r="AL16" s="110"/>
+      <c r="AM16" s="110"/>
+      <c r="AN16" s="110"/>
+      <c r="AO16" s="110"/>
+      <c r="AP16" s="110"/>
+      <c r="AQ16" s="110"/>
+      <c r="AR16" s="110"/>
+      <c r="AS16" s="110"/>
+      <c r="AT16" s="110"/>
+      <c r="AU16" s="110"/>
+      <c r="AV16" s="110"/>
+      <c r="AW16" s="110"/>
+      <c r="AX16" s="110"/>
+      <c r="AY16" s="110"/>
+      <c r="AZ16" s="111"/>
     </row>
     <row r="17" spans="1:52">
-      <c r="A17" s="141"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="135"/>
-      <c r="G17" s="135"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="143" t="s">
+      <c r="A17" s="124"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="126" t="s">
         <v>1374</v>
       </c>
-      <c r="J17" s="135"/>
-      <c r="K17" s="135"/>
-      <c r="L17" s="135"/>
-      <c r="M17" s="135"/>
-      <c r="N17" s="135"/>
-      <c r="O17" s="135"/>
-      <c r="P17" s="135"/>
-      <c r="Q17" s="135"/>
-      <c r="R17" s="135"/>
-      <c r="S17" s="135"/>
-      <c r="T17" s="135"/>
-      <c r="U17" s="135"/>
-      <c r="V17" s="135"/>
-      <c r="W17" s="135"/>
-      <c r="X17" s="135"/>
-      <c r="Y17" s="135"/>
-      <c r="Z17" s="135"/>
-      <c r="AA17" s="135"/>
-      <c r="AB17" s="135"/>
-      <c r="AC17" s="135"/>
-      <c r="AD17" s="136"/>
-      <c r="AE17" s="135"/>
-      <c r="AF17" s="135"/>
-      <c r="AG17" s="135"/>
-      <c r="AH17" s="135"/>
-      <c r="AI17" s="135"/>
-      <c r="AJ17" s="135"/>
-      <c r="AK17" s="135"/>
-      <c r="AL17" s="135"/>
-      <c r="AM17" s="135"/>
-      <c r="AN17" s="135"/>
-      <c r="AO17" s="135"/>
-      <c r="AP17" s="135"/>
-      <c r="AQ17" s="135"/>
-      <c r="AR17" s="135"/>
-      <c r="AS17" s="135"/>
-      <c r="AT17" s="135"/>
-      <c r="AU17" s="135"/>
-      <c r="AV17" s="135"/>
-      <c r="AW17" s="135"/>
-      <c r="AX17" s="135"/>
-      <c r="AY17" s="135"/>
-      <c r="AZ17" s="136"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="118"/>
+      <c r="R17" s="118"/>
+      <c r="S17" s="118"/>
+      <c r="T17" s="118"/>
+      <c r="U17" s="118"/>
+      <c r="V17" s="118"/>
+      <c r="W17" s="118"/>
+      <c r="X17" s="118"/>
+      <c r="Y17" s="118"/>
+      <c r="Z17" s="118"/>
+      <c r="AA17" s="118"/>
+      <c r="AB17" s="118"/>
+      <c r="AC17" s="118"/>
+      <c r="AD17" s="119"/>
+      <c r="AE17" s="118"/>
+      <c r="AF17" s="118"/>
+      <c r="AG17" s="118"/>
+      <c r="AH17" s="118"/>
+      <c r="AI17" s="118"/>
+      <c r="AJ17" s="118"/>
+      <c r="AK17" s="118"/>
+      <c r="AL17" s="118"/>
+      <c r="AM17" s="118"/>
+      <c r="AN17" s="118"/>
+      <c r="AO17" s="118"/>
+      <c r="AP17" s="118"/>
+      <c r="AQ17" s="118"/>
+      <c r="AR17" s="118"/>
+      <c r="AS17" s="118"/>
+      <c r="AT17" s="118"/>
+      <c r="AU17" s="118"/>
+      <c r="AV17" s="118"/>
+      <c r="AW17" s="118"/>
+      <c r="AX17" s="118"/>
+      <c r="AY17" s="118"/>
+      <c r="AZ17" s="119"/>
     </row>
     <row r="18" spans="1:52">
-      <c r="A18" s="141"/>
-      <c r="C18" s="144" t="s">
+      <c r="A18" s="124"/>
+      <c r="C18" s="127" t="s">
         <v>1375</v>
       </c>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="120" t="s">
+      <c r="D18" s="128"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="103" t="s">
         <v>1376</v>
       </c>
-      <c r="J18" s="145"/>
-      <c r="K18" s="145"/>
-      <c r="L18" s="145"/>
-      <c r="M18" s="145"/>
-      <c r="N18" s="145"/>
-      <c r="O18" s="145"/>
-      <c r="P18" s="145"/>
-      <c r="Q18" s="145"/>
-      <c r="R18" s="145"/>
-      <c r="S18" s="145"/>
-      <c r="T18" s="145"/>
-      <c r="U18" s="145"/>
-      <c r="V18" s="145"/>
-      <c r="W18" s="145"/>
-      <c r="X18" s="145"/>
-      <c r="Y18" s="145"/>
-      <c r="Z18" s="145"/>
-      <c r="AA18" s="145"/>
-      <c r="AB18" s="145"/>
-      <c r="AC18" s="145"/>
-      <c r="AD18" s="146"/>
-      <c r="AE18" s="147" t="s">
+      <c r="J18" s="128"/>
+      <c r="K18" s="128"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="128"/>
+      <c r="N18" s="128"/>
+      <c r="O18" s="128"/>
+      <c r="P18" s="128"/>
+      <c r="Q18" s="128"/>
+      <c r="R18" s="128"/>
+      <c r="S18" s="128"/>
+      <c r="T18" s="128"/>
+      <c r="U18" s="128"/>
+      <c r="V18" s="128"/>
+      <c r="W18" s="128"/>
+      <c r="X18" s="128"/>
+      <c r="Y18" s="128"/>
+      <c r="Z18" s="128"/>
+      <c r="AA18" s="128"/>
+      <c r="AB18" s="128"/>
+      <c r="AC18" s="128"/>
+      <c r="AD18" s="129"/>
+      <c r="AE18" s="130" t="s">
         <v>1377</v>
       </c>
-      <c r="AF18" s="145"/>
-      <c r="AG18" s="145"/>
-      <c r="AH18" s="145"/>
-      <c r="AI18" s="145"/>
-      <c r="AJ18" s="145"/>
-      <c r="AK18" s="145"/>
-      <c r="AL18" s="145"/>
-      <c r="AM18" s="145"/>
-      <c r="AN18" s="145"/>
-      <c r="AO18" s="145"/>
-      <c r="AP18" s="145"/>
-      <c r="AQ18" s="145"/>
-      <c r="AR18" s="145"/>
-      <c r="AS18" s="145"/>
-      <c r="AT18" s="145"/>
-      <c r="AU18" s="145"/>
-      <c r="AV18" s="145"/>
-      <c r="AW18" s="145"/>
-      <c r="AX18" s="145"/>
-      <c r="AY18" s="145"/>
-      <c r="AZ18" s="146"/>
+      <c r="AF18" s="128"/>
+      <c r="AG18" s="128"/>
+      <c r="AH18" s="128"/>
+      <c r="AI18" s="128"/>
+      <c r="AJ18" s="128"/>
+      <c r="AK18" s="128"/>
+      <c r="AL18" s="128"/>
+      <c r="AM18" s="128"/>
+      <c r="AN18" s="128"/>
+      <c r="AO18" s="128"/>
+      <c r="AP18" s="128"/>
+      <c r="AQ18" s="128"/>
+      <c r="AR18" s="128"/>
+      <c r="AS18" s="128"/>
+      <c r="AT18" s="128"/>
+      <c r="AU18" s="128"/>
+      <c r="AV18" s="128"/>
+      <c r="AW18" s="128"/>
+      <c r="AX18" s="128"/>
+      <c r="AY18" s="128"/>
+      <c r="AZ18" s="129"/>
     </row>
     <row r="19" spans="1:52">
-      <c r="A19" s="141"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="148" t="s">
+      <c r="A19" s="124"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="131" t="s">
         <v>1378</v>
       </c>
-      <c r="J19" s="135"/>
-      <c r="K19" s="135"/>
-      <c r="L19" s="135"/>
-      <c r="M19" s="135"/>
-      <c r="N19" s="135"/>
-      <c r="O19" s="135"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="135"/>
-      <c r="R19" s="135"/>
-      <c r="S19" s="135"/>
-      <c r="T19" s="135"/>
-      <c r="U19" s="135"/>
-      <c r="V19" s="135"/>
-      <c r="W19" s="135"/>
-      <c r="X19" s="135"/>
-      <c r="Y19" s="135"/>
-      <c r="Z19" s="135"/>
-      <c r="AA19" s="135"/>
-      <c r="AB19" s="135"/>
-      <c r="AC19" s="135"/>
-      <c r="AD19" s="136"/>
-      <c r="AE19" s="135"/>
-      <c r="AF19" s="135"/>
-      <c r="AG19" s="135"/>
-      <c r="AH19" s="135"/>
-      <c r="AI19" s="135"/>
-      <c r="AJ19" s="135"/>
-      <c r="AK19" s="135"/>
-      <c r="AL19" s="135"/>
-      <c r="AM19" s="135"/>
-      <c r="AN19" s="135"/>
-      <c r="AO19" s="135"/>
-      <c r="AP19" s="135"/>
-      <c r="AQ19" s="135"/>
-      <c r="AR19" s="135"/>
-      <c r="AS19" s="135"/>
-      <c r="AT19" s="135"/>
-      <c r="AU19" s="135"/>
-      <c r="AV19" s="135"/>
-      <c r="AW19" s="135"/>
-      <c r="AX19" s="135"/>
-      <c r="AY19" s="135"/>
-      <c r="AZ19" s="136"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
+      <c r="N19" s="118"/>
+      <c r="O19" s="118"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="118"/>
+      <c r="R19" s="118"/>
+      <c r="S19" s="118"/>
+      <c r="T19" s="118"/>
+      <c r="U19" s="118"/>
+      <c r="V19" s="118"/>
+      <c r="W19" s="118"/>
+      <c r="X19" s="118"/>
+      <c r="Y19" s="118"/>
+      <c r="Z19" s="118"/>
+      <c r="AA19" s="118"/>
+      <c r="AB19" s="118"/>
+      <c r="AC19" s="118"/>
+      <c r="AD19" s="119"/>
+      <c r="AE19" s="118"/>
+      <c r="AF19" s="118"/>
+      <c r="AG19" s="118"/>
+      <c r="AH19" s="118"/>
+      <c r="AI19" s="118"/>
+      <c r="AJ19" s="118"/>
+      <c r="AK19" s="118"/>
+      <c r="AL19" s="118"/>
+      <c r="AM19" s="118"/>
+      <c r="AN19" s="118"/>
+      <c r="AO19" s="118"/>
+      <c r="AP19" s="118"/>
+      <c r="AQ19" s="118"/>
+      <c r="AR19" s="118"/>
+      <c r="AS19" s="118"/>
+      <c r="AT19" s="118"/>
+      <c r="AU19" s="118"/>
+      <c r="AV19" s="118"/>
+      <c r="AW19" s="118"/>
+      <c r="AX19" s="118"/>
+      <c r="AY19" s="118"/>
+      <c r="AZ19" s="119"/>
     </row>
     <row r="20" spans="1:52">
-      <c r="A20" s="141"/>
-      <c r="C20" s="126" t="s">
+      <c r="A20" s="124"/>
+      <c r="C20" s="109" t="s">
         <v>1379</v>
       </c>
-      <c r="D20" s="127"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="127"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="127"/>
-      <c r="I20" s="120" t="s">
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="103" t="s">
         <v>1380</v>
       </c>
-      <c r="J20" s="127"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="127"/>
-      <c r="M20" s="127"/>
-      <c r="N20" s="127"/>
-      <c r="O20" s="127"/>
-      <c r="P20" s="127"/>
-      <c r="Q20" s="127"/>
-      <c r="R20" s="127"/>
-      <c r="S20" s="127"/>
-      <c r="T20" s="127"/>
-      <c r="U20" s="127"/>
-      <c r="V20" s="127"/>
-      <c r="W20" s="127"/>
-      <c r="X20" s="127"/>
-      <c r="Y20" s="127"/>
-      <c r="Z20" s="127"/>
-      <c r="AA20" s="127"/>
-      <c r="AB20" s="127"/>
-      <c r="AC20" s="127"/>
-      <c r="AD20" s="128"/>
-      <c r="AE20" s="142" t="s">
+      <c r="J20" s="110"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="110"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="110"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="110"/>
+      <c r="W20" s="110"/>
+      <c r="X20" s="110"/>
+      <c r="Y20" s="110"/>
+      <c r="Z20" s="110"/>
+      <c r="AA20" s="110"/>
+      <c r="AB20" s="110"/>
+      <c r="AC20" s="110"/>
+      <c r="AD20" s="111"/>
+      <c r="AE20" s="125" t="s">
         <v>1381</v>
       </c>
-      <c r="AF20" s="127"/>
-      <c r="AG20" s="127"/>
-      <c r="AH20" s="127"/>
-      <c r="AI20" s="127"/>
-      <c r="AJ20" s="127"/>
-      <c r="AK20" s="127"/>
-      <c r="AL20" s="127"/>
-      <c r="AM20" s="127"/>
-      <c r="AN20" s="127"/>
-      <c r="AO20" s="127"/>
-      <c r="AP20" s="127"/>
-      <c r="AQ20" s="127"/>
-      <c r="AR20" s="127"/>
-      <c r="AS20" s="127"/>
-      <c r="AT20" s="127"/>
-      <c r="AU20" s="127"/>
-      <c r="AV20" s="127"/>
-      <c r="AW20" s="127"/>
-      <c r="AX20" s="127"/>
-      <c r="AY20" s="127"/>
-      <c r="AZ20" s="128"/>
+      <c r="AF20" s="110"/>
+      <c r="AG20" s="110"/>
+      <c r="AH20" s="110"/>
+      <c r="AI20" s="110"/>
+      <c r="AJ20" s="110"/>
+      <c r="AK20" s="110"/>
+      <c r="AL20" s="110"/>
+      <c r="AM20" s="110"/>
+      <c r="AN20" s="110"/>
+      <c r="AO20" s="110"/>
+      <c r="AP20" s="110"/>
+      <c r="AQ20" s="110"/>
+      <c r="AR20" s="110"/>
+      <c r="AS20" s="110"/>
+      <c r="AT20" s="110"/>
+      <c r="AU20" s="110"/>
+      <c r="AV20" s="110"/>
+      <c r="AW20" s="110"/>
+      <c r="AX20" s="110"/>
+      <c r="AY20" s="110"/>
+      <c r="AZ20" s="111"/>
     </row>
     <row r="21" spans="1:52">
-      <c r="A21" s="141"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="137" t="s">
+      <c r="A21" s="124"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="120" t="s">
         <v>1382</v>
       </c>
-      <c r="J21" s="135"/>
-      <c r="K21" s="135"/>
-      <c r="L21" s="135"/>
-      <c r="M21" s="135"/>
-      <c r="N21" s="135"/>
-      <c r="O21" s="135"/>
-      <c r="P21" s="135"/>
-      <c r="Q21" s="135"/>
-      <c r="R21" s="135"/>
-      <c r="S21" s="135"/>
-      <c r="T21" s="135"/>
-      <c r="U21" s="135"/>
-      <c r="V21" s="135"/>
-      <c r="W21" s="135"/>
-      <c r="X21" s="135"/>
-      <c r="Y21" s="135"/>
-      <c r="Z21" s="135"/>
-      <c r="AA21" s="135"/>
-      <c r="AB21" s="135"/>
-      <c r="AC21" s="135"/>
-      <c r="AD21" s="136"/>
-      <c r="AE21" s="135"/>
-      <c r="AF21" s="135"/>
-      <c r="AG21" s="135"/>
-      <c r="AH21" s="135"/>
-      <c r="AI21" s="135"/>
-      <c r="AJ21" s="135"/>
-      <c r="AK21" s="135"/>
-      <c r="AL21" s="135"/>
-      <c r="AM21" s="135"/>
-      <c r="AN21" s="135"/>
-      <c r="AO21" s="135"/>
-      <c r="AP21" s="135"/>
-      <c r="AQ21" s="135"/>
-      <c r="AR21" s="135"/>
-      <c r="AS21" s="135"/>
-      <c r="AT21" s="135"/>
-      <c r="AU21" s="135"/>
-      <c r="AV21" s="135"/>
-      <c r="AW21" s="135"/>
-      <c r="AX21" s="135"/>
-      <c r="AY21" s="135"/>
-      <c r="AZ21" s="136"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="118"/>
+      <c r="O21" s="118"/>
+      <c r="P21" s="118"/>
+      <c r="Q21" s="118"/>
+      <c r="R21" s="118"/>
+      <c r="S21" s="118"/>
+      <c r="T21" s="118"/>
+      <c r="U21" s="118"/>
+      <c r="V21" s="118"/>
+      <c r="W21" s="118"/>
+      <c r="X21" s="118"/>
+      <c r="Y21" s="118"/>
+      <c r="Z21" s="118"/>
+      <c r="AA21" s="118"/>
+      <c r="AB21" s="118"/>
+      <c r="AC21" s="118"/>
+      <c r="AD21" s="119"/>
+      <c r="AE21" s="118"/>
+      <c r="AF21" s="118"/>
+      <c r="AG21" s="118"/>
+      <c r="AH21" s="118"/>
+      <c r="AI21" s="118"/>
+      <c r="AJ21" s="118"/>
+      <c r="AK21" s="118"/>
+      <c r="AL21" s="118"/>
+      <c r="AM21" s="118"/>
+      <c r="AN21" s="118"/>
+      <c r="AO21" s="118"/>
+      <c r="AP21" s="118"/>
+      <c r="AQ21" s="118"/>
+      <c r="AR21" s="118"/>
+      <c r="AS21" s="118"/>
+      <c r="AT21" s="118"/>
+      <c r="AU21" s="118"/>
+      <c r="AV21" s="118"/>
+      <c r="AW21" s="118"/>
+      <c r="AX21" s="118"/>
+      <c r="AY21" s="118"/>
+      <c r="AZ21" s="119"/>
     </row>
     <row r="22" spans="1:52">
-      <c r="A22" s="141"/>
+      <c r="A22" s="124"/>
     </row>
     <row r="23" spans="1:52">
-      <c r="A23" s="141"/>
-      <c r="B23" s="118" t="s">
+      <c r="A23" s="124"/>
+      <c r="B23" s="101" t="s">
         <v>1383</v>
       </c>
     </row>
     <row r="24" spans="1:52">
-      <c r="C24" s="138" t="s">
+      <c r="C24" s="121" t="s">
         <v>1384</v>
       </c>
     </row>
     <row r="26" spans="1:52" ht="15" thickBot="1">
-      <c r="C26" s="139" t="s">
+      <c r="C26" s="122" t="s">
         <v>1385</v>
       </c>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="124"/>
-      <c r="G26" s="124"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="149"/>
-      <c r="J26" s="150" t="s">
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="133" t="s">
         <v>1361</v>
       </c>
-      <c r="K26" s="151"/>
-      <c r="L26" s="151"/>
-      <c r="M26" s="152"/>
-      <c r="N26" s="140" t="s">
+      <c r="K26" s="134"/>
+      <c r="L26" s="134"/>
+      <c r="M26" s="135"/>
+      <c r="N26" s="123" t="s">
         <v>1386</v>
       </c>
-      <c r="O26" s="124"/>
-      <c r="P26" s="124"/>
-      <c r="Q26" s="124"/>
-      <c r="R26" s="153" t="s">
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="136" t="s">
         <v>1365</v>
       </c>
-      <c r="S26" s="124"/>
-      <c r="T26" s="124"/>
-      <c r="U26" s="125"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="107"/>
+      <c r="U26" s="108"/>
     </row>
     <row r="27" spans="1:52" ht="15" thickTop="1">
-      <c r="C27" s="134" t="s">
+      <c r="C27" s="117" t="s">
         <v>1371</v>
       </c>
-      <c r="D27" s="135"/>
-      <c r="E27" s="135"/>
-      <c r="F27" s="135"/>
-      <c r="G27" s="135"/>
-      <c r="H27" s="135"/>
-      <c r="I27" s="154"/>
-      <c r="J27" s="155" t="s">
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="138" t="s">
         <v>1387</v>
       </c>
-      <c r="K27" s="156"/>
-      <c r="L27" s="156"/>
-      <c r="M27" s="157"/>
-      <c r="N27" s="135" t="s">
+      <c r="K27" s="139"/>
+      <c r="L27" s="139"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="118" t="s">
         <v>1388</v>
       </c>
-      <c r="O27" s="135"/>
-      <c r="P27" s="135"/>
-      <c r="Q27" s="135"/>
-      <c r="R27" s="134" t="s">
+      <c r="O27" s="118"/>
+      <c r="P27" s="118"/>
+      <c r="Q27" s="118"/>
+      <c r="R27" s="117" t="s">
         <v>1388</v>
       </c>
-      <c r="S27" s="135"/>
-      <c r="T27" s="135"/>
-      <c r="U27" s="136"/>
+      <c r="S27" s="118"/>
+      <c r="T27" s="118"/>
+      <c r="U27" s="119"/>
     </row>
     <row r="28" spans="1:52">
-      <c r="C28" s="134" t="s">
+      <c r="C28" s="117" t="s">
         <v>1375</v>
       </c>
-      <c r="D28" s="135"/>
-      <c r="E28" s="135"/>
-      <c r="F28" s="135"/>
-      <c r="G28" s="135"/>
-      <c r="H28" s="135"/>
-      <c r="I28" s="132"/>
-      <c r="J28" s="155" t="s">
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="118"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="138" t="s">
         <v>1388</v>
       </c>
-      <c r="K28" s="156"/>
-      <c r="L28" s="156"/>
-      <c r="M28" s="157"/>
-      <c r="N28" s="135" t="s">
+      <c r="K28" s="139"/>
+      <c r="L28" s="139"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="118" t="s">
         <v>1387</v>
       </c>
-      <c r="O28" s="135"/>
-      <c r="P28" s="135"/>
-      <c r="Q28" s="135"/>
-      <c r="R28" s="134" t="s">
+      <c r="O28" s="118"/>
+      <c r="P28" s="118"/>
+      <c r="Q28" s="118"/>
+      <c r="R28" s="117" t="s">
         <v>1388</v>
       </c>
-      <c r="S28" s="135"/>
-      <c r="T28" s="135"/>
-      <c r="U28" s="136"/>
+      <c r="S28" s="118"/>
+      <c r="T28" s="118"/>
+      <c r="U28" s="119"/>
     </row>
     <row r="29" spans="1:52">
-      <c r="C29" s="134" t="s">
+      <c r="C29" s="117" t="s">
         <v>1379</v>
       </c>
-      <c r="D29" s="135"/>
-      <c r="E29" s="135"/>
-      <c r="F29" s="135"/>
-      <c r="G29" s="135"/>
-      <c r="H29" s="135"/>
-      <c r="I29" s="136"/>
-      <c r="J29" s="155" t="s">
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="118"/>
+      <c r="I29" s="119"/>
+      <c r="J29" s="138" t="s">
         <v>1387</v>
       </c>
-      <c r="K29" s="156"/>
-      <c r="L29" s="156"/>
-      <c r="M29" s="157"/>
-      <c r="N29" s="135" t="s">
+      <c r="K29" s="139"/>
+      <c r="L29" s="139"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="118" t="s">
         <v>1387</v>
       </c>
-      <c r="O29" s="135"/>
-      <c r="P29" s="135"/>
-      <c r="Q29" s="135"/>
-      <c r="R29" s="134" t="s">
+      <c r="O29" s="118"/>
+      <c r="P29" s="118"/>
+      <c r="Q29" s="118"/>
+      <c r="R29" s="117" t="s">
         <v>1388</v>
       </c>
-      <c r="S29" s="135"/>
-      <c r="T29" s="135"/>
-      <c r="U29" s="136"/>
-      <c r="AC29" s="158"/>
+      <c r="S29" s="118"/>
+      <c r="T29" s="118"/>
+      <c r="U29" s="119"/>
+      <c r="AC29" s="141"/>
     </row>
     <row r="31" spans="1:52">
-      <c r="B31" s="121" t="s">
+      <c r="B31" s="104" t="s">
         <v>1389</v>
       </c>
     </row>
     <row r="32" spans="1:52">
-      <c r="C32" s="138" t="s">
+      <c r="C32" s="121" t="s">
         <v>1390</v>
       </c>
     </row>
     <row r="34" spans="1:70">
-      <c r="C34" s="121" t="s">
+      <c r="C34" s="104" t="s">
         <v>1391</v>
       </c>
-      <c r="D34" s="138"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="121"/>
     </row>
     <row r="36" spans="1:70">
-      <c r="D36" s="118" t="s">
+      <c r="D36" s="101" t="s">
         <v>1392</v>
       </c>
     </row>
     <row r="37" spans="1:70">
-      <c r="D37" s="122"/>
-      <c r="E37" s="120" t="s">
+      <c r="D37" s="105"/>
+      <c r="E37" s="103" t="s">
         <v>1393</v>
       </c>
     </row>
     <row r="38" spans="1:70">
-      <c r="D38" s="122"/>
+      <c r="D38" s="105"/>
     </row>
     <row r="39" spans="1:70" ht="15" thickBot="1">
-      <c r="E39" s="123" t="s">
+      <c r="E39" s="106" t="s">
         <v>1394</v>
       </c>
-      <c r="F39" s="124"/>
-      <c r="G39" s="124"/>
-      <c r="H39" s="123" t="s">
+      <c r="F39" s="107"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="106" t="s">
         <v>1395</v>
       </c>
-      <c r="I39" s="124"/>
-      <c r="J39" s="124"/>
-      <c r="K39" s="124"/>
-      <c r="L39" s="124"/>
-      <c r="M39" s="124"/>
-      <c r="N39" s="124"/>
-      <c r="O39" s="124"/>
-      <c r="P39" s="124"/>
-      <c r="Q39" s="124"/>
-      <c r="R39" s="125"/>
-      <c r="S39" s="159" t="s">
+      <c r="I39" s="107"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="107"/>
+      <c r="L39" s="107"/>
+      <c r="M39" s="107"/>
+      <c r="N39" s="107"/>
+      <c r="O39" s="107"/>
+      <c r="P39" s="107"/>
+      <c r="Q39" s="107"/>
+      <c r="R39" s="108"/>
+      <c r="S39" s="142" t="s">
         <v>1396</v>
       </c>
-      <c r="T39" s="124"/>
-      <c r="U39" s="124"/>
-      <c r="V39" s="124"/>
-      <c r="W39" s="124"/>
-      <c r="X39" s="124"/>
-      <c r="Y39" s="124"/>
-      <c r="Z39" s="124"/>
-      <c r="AA39" s="124"/>
-      <c r="AB39" s="124"/>
-      <c r="AC39" s="124"/>
-      <c r="AD39" s="124"/>
-      <c r="AE39" s="124"/>
-      <c r="AF39" s="124"/>
-      <c r="AG39" s="124"/>
-      <c r="AH39" s="124"/>
-      <c r="AI39" s="124"/>
-      <c r="AJ39" s="124"/>
-      <c r="AK39" s="124"/>
-      <c r="AL39" s="124"/>
-      <c r="AM39" s="123" t="s">
+      <c r="T39" s="107"/>
+      <c r="U39" s="107"/>
+      <c r="V39" s="107"/>
+      <c r="W39" s="107"/>
+      <c r="X39" s="107"/>
+      <c r="Y39" s="107"/>
+      <c r="Z39" s="107"/>
+      <c r="AA39" s="107"/>
+      <c r="AB39" s="107"/>
+      <c r="AC39" s="107"/>
+      <c r="AD39" s="107"/>
+      <c r="AE39" s="107"/>
+      <c r="AF39" s="107"/>
+      <c r="AG39" s="107"/>
+      <c r="AH39" s="107"/>
+      <c r="AI39" s="107"/>
+      <c r="AJ39" s="107"/>
+      <c r="AK39" s="107"/>
+      <c r="AL39" s="107"/>
+      <c r="AM39" s="106" t="s">
         <v>1397</v>
       </c>
-      <c r="AN39" s="124"/>
-      <c r="AO39" s="124"/>
-      <c r="AP39" s="124"/>
-      <c r="AQ39" s="124"/>
-      <c r="AR39" s="124"/>
-      <c r="AS39" s="124"/>
-      <c r="AT39" s="124"/>
-      <c r="AU39" s="124"/>
-      <c r="AV39" s="124"/>
-      <c r="AW39" s="124"/>
-      <c r="AX39" s="124"/>
-      <c r="AY39" s="124"/>
-      <c r="AZ39" s="124"/>
-      <c r="BA39" s="124"/>
-      <c r="BB39" s="124"/>
-      <c r="BC39" s="124"/>
-      <c r="BD39" s="124"/>
-      <c r="BE39" s="124"/>
-      <c r="BF39" s="124"/>
-      <c r="BG39" s="124"/>
-      <c r="BH39" s="124"/>
-      <c r="BI39" s="124"/>
-      <c r="BJ39" s="124"/>
-      <c r="BK39" s="124"/>
-      <c r="BL39" s="124"/>
-      <c r="BM39" s="124"/>
-      <c r="BN39" s="124"/>
-      <c r="BO39" s="124"/>
-      <c r="BP39" s="124"/>
-      <c r="BQ39" s="124"/>
-      <c r="BR39" s="125"/>
+      <c r="AN39" s="107"/>
+      <c r="AO39" s="107"/>
+      <c r="AP39" s="107"/>
+      <c r="AQ39" s="107"/>
+      <c r="AR39" s="107"/>
+      <c r="AS39" s="107"/>
+      <c r="AT39" s="107"/>
+      <c r="AU39" s="107"/>
+      <c r="AV39" s="107"/>
+      <c r="AW39" s="107"/>
+      <c r="AX39" s="107"/>
+      <c r="AY39" s="107"/>
+      <c r="AZ39" s="107"/>
+      <c r="BA39" s="107"/>
+      <c r="BB39" s="107"/>
+      <c r="BC39" s="107"/>
+      <c r="BD39" s="107"/>
+      <c r="BE39" s="107"/>
+      <c r="BF39" s="107"/>
+      <c r="BG39" s="107"/>
+      <c r="BH39" s="107"/>
+      <c r="BI39" s="107"/>
+      <c r="BJ39" s="107"/>
+      <c r="BK39" s="107"/>
+      <c r="BL39" s="107"/>
+      <c r="BM39" s="107"/>
+      <c r="BN39" s="107"/>
+      <c r="BO39" s="107"/>
+      <c r="BP39" s="107"/>
+      <c r="BQ39" s="107"/>
+      <c r="BR39" s="108"/>
     </row>
     <row r="40" spans="1:70" ht="15" thickTop="1">
-      <c r="A40" s="141"/>
-      <c r="E40" s="134" t="s">
+      <c r="A40" s="124"/>
+      <c r="E40" s="117" t="s">
         <v>1398</v>
       </c>
-      <c r="F40" s="135"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="137" t="s">
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="120" t="s">
         <v>1399</v>
       </c>
-      <c r="I40" s="135"/>
-      <c r="J40" s="135"/>
-      <c r="K40" s="135"/>
-      <c r="L40" s="135"/>
-      <c r="M40" s="135"/>
-      <c r="N40" s="135"/>
-      <c r="O40" s="135"/>
-      <c r="P40" s="135"/>
-      <c r="Q40" s="135"/>
-      <c r="R40" s="136"/>
-      <c r="S40" s="160" t="s">
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="118"/>
+      <c r="L40" s="118"/>
+      <c r="M40" s="118"/>
+      <c r="N40" s="118"/>
+      <c r="O40" s="118"/>
+      <c r="P40" s="118"/>
+      <c r="Q40" s="118"/>
+      <c r="R40" s="119"/>
+      <c r="S40" s="143" t="s">
         <v>1400</v>
       </c>
-      <c r="T40" s="135"/>
-      <c r="U40" s="135"/>
-      <c r="V40" s="135"/>
-      <c r="W40" s="135"/>
-      <c r="X40" s="135"/>
-      <c r="Y40" s="135"/>
-      <c r="Z40" s="135"/>
-      <c r="AA40" s="135"/>
-      <c r="AB40" s="135"/>
-      <c r="AC40" s="135"/>
-      <c r="AD40" s="135"/>
-      <c r="AE40" s="135"/>
-      <c r="AF40" s="135"/>
-      <c r="AG40" s="135"/>
-      <c r="AH40" s="135"/>
-      <c r="AI40" s="135"/>
-      <c r="AJ40" s="135"/>
-      <c r="AK40" s="135"/>
-      <c r="AL40" s="135"/>
-      <c r="AM40" s="137" t="s">
+      <c r="T40" s="118"/>
+      <c r="U40" s="118"/>
+      <c r="V40" s="118"/>
+      <c r="W40" s="118"/>
+      <c r="X40" s="118"/>
+      <c r="Y40" s="118"/>
+      <c r="Z40" s="118"/>
+      <c r="AA40" s="118"/>
+      <c r="AB40" s="118"/>
+      <c r="AC40" s="118"/>
+      <c r="AD40" s="118"/>
+      <c r="AE40" s="118"/>
+      <c r="AF40" s="118"/>
+      <c r="AG40" s="118"/>
+      <c r="AH40" s="118"/>
+      <c r="AI40" s="118"/>
+      <c r="AJ40" s="118"/>
+      <c r="AK40" s="118"/>
+      <c r="AL40" s="118"/>
+      <c r="AM40" s="120" t="s">
         <v>1401</v>
       </c>
-      <c r="AN40" s="135"/>
-      <c r="AO40" s="135"/>
-      <c r="AP40" s="135"/>
-      <c r="AQ40" s="135"/>
-      <c r="AR40" s="135"/>
-      <c r="AS40" s="135"/>
-      <c r="AT40" s="135"/>
-      <c r="AU40" s="135"/>
-      <c r="AV40" s="135"/>
-      <c r="AW40" s="135"/>
-      <c r="AX40" s="135"/>
-      <c r="AY40" s="135"/>
-      <c r="AZ40" s="135"/>
-      <c r="BA40" s="135"/>
-      <c r="BB40" s="135"/>
-      <c r="BC40" s="135"/>
-      <c r="BD40" s="135"/>
-      <c r="BE40" s="135"/>
-      <c r="BF40" s="135"/>
-      <c r="BG40" s="135"/>
-      <c r="BH40" s="135"/>
-      <c r="BI40" s="135"/>
-      <c r="BJ40" s="135"/>
-      <c r="BK40" s="135"/>
-      <c r="BL40" s="135"/>
-      <c r="BM40" s="135"/>
-      <c r="BN40" s="135"/>
-      <c r="BO40" s="135"/>
-      <c r="BP40" s="135"/>
-      <c r="BQ40" s="135"/>
-      <c r="BR40" s="136"/>
+      <c r="AN40" s="118"/>
+      <c r="AO40" s="118"/>
+      <c r="AP40" s="118"/>
+      <c r="AQ40" s="118"/>
+      <c r="AR40" s="118"/>
+      <c r="AS40" s="118"/>
+      <c r="AT40" s="118"/>
+      <c r="AU40" s="118"/>
+      <c r="AV40" s="118"/>
+      <c r="AW40" s="118"/>
+      <c r="AX40" s="118"/>
+      <c r="AY40" s="118"/>
+      <c r="AZ40" s="118"/>
+      <c r="BA40" s="118"/>
+      <c r="BB40" s="118"/>
+      <c r="BC40" s="118"/>
+      <c r="BD40" s="118"/>
+      <c r="BE40" s="118"/>
+      <c r="BF40" s="118"/>
+      <c r="BG40" s="118"/>
+      <c r="BH40" s="118"/>
+      <c r="BI40" s="118"/>
+      <c r="BJ40" s="118"/>
+      <c r="BK40" s="118"/>
+      <c r="BL40" s="118"/>
+      <c r="BM40" s="118"/>
+      <c r="BN40" s="118"/>
+      <c r="BO40" s="118"/>
+      <c r="BP40" s="118"/>
+      <c r="BQ40" s="118"/>
+      <c r="BR40" s="119"/>
     </row>
     <row r="41" spans="1:70">
-      <c r="A41" s="141"/>
-      <c r="E41" s="134" t="s">
+      <c r="A41" s="124"/>
+      <c r="E41" s="117" t="s">
         <v>1402</v>
       </c>
-      <c r="F41" s="135"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="137" t="s">
+      <c r="F41" s="118"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="120" t="s">
         <v>1403</v>
       </c>
-      <c r="I41" s="135"/>
-      <c r="J41" s="135"/>
-      <c r="K41" s="135"/>
-      <c r="L41" s="135"/>
-      <c r="M41" s="135"/>
-      <c r="N41" s="135"/>
-      <c r="O41" s="135"/>
-      <c r="P41" s="135"/>
-      <c r="Q41" s="135"/>
-      <c r="R41" s="136"/>
-      <c r="S41" s="160" t="s">
+      <c r="I41" s="118"/>
+      <c r="J41" s="118"/>
+      <c r="K41" s="118"/>
+      <c r="L41" s="118"/>
+      <c r="M41" s="118"/>
+      <c r="N41" s="118"/>
+      <c r="O41" s="118"/>
+      <c r="P41" s="118"/>
+      <c r="Q41" s="118"/>
+      <c r="R41" s="119"/>
+      <c r="S41" s="143" t="s">
         <v>1404</v>
       </c>
-      <c r="T41" s="135"/>
-      <c r="U41" s="135"/>
-      <c r="V41" s="135"/>
-      <c r="W41" s="135"/>
-      <c r="X41" s="135"/>
-      <c r="Y41" s="135"/>
-      <c r="Z41" s="135"/>
-      <c r="AA41" s="135"/>
-      <c r="AB41" s="135"/>
-      <c r="AC41" s="135"/>
-      <c r="AD41" s="135"/>
-      <c r="AE41" s="135"/>
-      <c r="AF41" s="135"/>
-      <c r="AG41" s="135"/>
-      <c r="AH41" s="135"/>
-      <c r="AI41" s="135"/>
-      <c r="AJ41" s="135"/>
-      <c r="AK41" s="135"/>
-      <c r="AL41" s="135"/>
-      <c r="AM41" s="137" t="s">
+      <c r="T41" s="118"/>
+      <c r="U41" s="118"/>
+      <c r="V41" s="118"/>
+      <c r="W41" s="118"/>
+      <c r="X41" s="118"/>
+      <c r="Y41" s="118"/>
+      <c r="Z41" s="118"/>
+      <c r="AA41" s="118"/>
+      <c r="AB41" s="118"/>
+      <c r="AC41" s="118"/>
+      <c r="AD41" s="118"/>
+      <c r="AE41" s="118"/>
+      <c r="AF41" s="118"/>
+      <c r="AG41" s="118"/>
+      <c r="AH41" s="118"/>
+      <c r="AI41" s="118"/>
+      <c r="AJ41" s="118"/>
+      <c r="AK41" s="118"/>
+      <c r="AL41" s="118"/>
+      <c r="AM41" s="120" t="s">
         <v>1405</v>
       </c>
-      <c r="AN41" s="135"/>
-      <c r="AO41" s="135"/>
-      <c r="AP41" s="135"/>
-      <c r="AQ41" s="135"/>
-      <c r="AR41" s="135"/>
-      <c r="AS41" s="135"/>
-      <c r="AT41" s="135"/>
-      <c r="AU41" s="135"/>
-      <c r="AV41" s="135"/>
-      <c r="AW41" s="135"/>
-      <c r="AX41" s="135"/>
-      <c r="AY41" s="135"/>
-      <c r="AZ41" s="135"/>
-      <c r="BA41" s="135"/>
-      <c r="BB41" s="135"/>
-      <c r="BC41" s="135"/>
-      <c r="BD41" s="135"/>
-      <c r="BE41" s="135"/>
-      <c r="BF41" s="135"/>
-      <c r="BG41" s="135"/>
-      <c r="BH41" s="135"/>
-      <c r="BI41" s="135"/>
-      <c r="BJ41" s="135"/>
-      <c r="BK41" s="135"/>
-      <c r="BL41" s="135"/>
-      <c r="BM41" s="135"/>
-      <c r="BN41" s="135"/>
-      <c r="BO41" s="135"/>
-      <c r="BP41" s="135"/>
-      <c r="BQ41" s="135"/>
-      <c r="BR41" s="136"/>
+      <c r="AN41" s="118"/>
+      <c r="AO41" s="118"/>
+      <c r="AP41" s="118"/>
+      <c r="AQ41" s="118"/>
+      <c r="AR41" s="118"/>
+      <c r="AS41" s="118"/>
+      <c r="AT41" s="118"/>
+      <c r="AU41" s="118"/>
+      <c r="AV41" s="118"/>
+      <c r="AW41" s="118"/>
+      <c r="AX41" s="118"/>
+      <c r="AY41" s="118"/>
+      <c r="AZ41" s="118"/>
+      <c r="BA41" s="118"/>
+      <c r="BB41" s="118"/>
+      <c r="BC41" s="118"/>
+      <c r="BD41" s="118"/>
+      <c r="BE41" s="118"/>
+      <c r="BF41" s="118"/>
+      <c r="BG41" s="118"/>
+      <c r="BH41" s="118"/>
+      <c r="BI41" s="118"/>
+      <c r="BJ41" s="118"/>
+      <c r="BK41" s="118"/>
+      <c r="BL41" s="118"/>
+      <c r="BM41" s="118"/>
+      <c r="BN41" s="118"/>
+      <c r="BO41" s="118"/>
+      <c r="BP41" s="118"/>
+      <c r="BQ41" s="118"/>
+      <c r="BR41" s="119"/>
     </row>
     <row r="42" spans="1:70">
-      <c r="A42" s="141"/>
+      <c r="A42" s="124"/>
     </row>
     <row r="43" spans="1:70">
-      <c r="A43" s="141"/>
-      <c r="D43" s="118" t="s">
+      <c r="A43" s="124"/>
+      <c r="D43" s="101" t="s">
         <v>1406</v>
       </c>
     </row>
     <row r="44" spans="1:70">
-      <c r="A44" s="141"/>
-      <c r="D44" s="122"/>
-      <c r="E44" s="120" t="s">
+      <c r="A44" s="124"/>
+      <c r="D44" s="105"/>
+      <c r="E44" s="103" t="s">
         <v>1407</v>
       </c>
     </row>
     <row r="45" spans="1:70">
-      <c r="A45" s="141"/>
-      <c r="D45" s="122"/>
+      <c r="A45" s="124"/>
+      <c r="D45" s="105"/>
     </row>
     <row r="46" spans="1:70" ht="15" thickBot="1">
-      <c r="A46" s="141"/>
-      <c r="E46" s="123" t="s">
+      <c r="A46" s="124"/>
+      <c r="E46" s="106" t="s">
         <v>1394</v>
       </c>
-      <c r="F46" s="124"/>
-      <c r="G46" s="124"/>
-      <c r="H46" s="123" t="s">
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="106" t="s">
         <v>1395</v>
       </c>
-      <c r="I46" s="124"/>
-      <c r="J46" s="124"/>
-      <c r="K46" s="124"/>
-      <c r="L46" s="124"/>
-      <c r="M46" s="124"/>
-      <c r="N46" s="124"/>
-      <c r="O46" s="124"/>
-      <c r="P46" s="124"/>
-      <c r="Q46" s="124"/>
-      <c r="R46" s="125"/>
-      <c r="S46" s="159" t="s">
+      <c r="I46" s="107"/>
+      <c r="J46" s="107"/>
+      <c r="K46" s="107"/>
+      <c r="L46" s="107"/>
+      <c r="M46" s="107"/>
+      <c r="N46" s="107"/>
+      <c r="O46" s="107"/>
+      <c r="P46" s="107"/>
+      <c r="Q46" s="107"/>
+      <c r="R46" s="108"/>
+      <c r="S46" s="142" t="s">
         <v>1408</v>
       </c>
-      <c r="T46" s="124"/>
-      <c r="U46" s="124"/>
-      <c r="V46" s="124"/>
-      <c r="W46" s="124"/>
-      <c r="X46" s="124"/>
-      <c r="Y46" s="124"/>
-      <c r="Z46" s="124"/>
-      <c r="AA46" s="124"/>
-      <c r="AB46" s="124"/>
-      <c r="AC46" s="124"/>
-      <c r="AD46" s="124"/>
-      <c r="AE46" s="124"/>
-      <c r="AF46" s="124"/>
-      <c r="AG46" s="124"/>
-      <c r="AH46" s="124"/>
-      <c r="AI46" s="124"/>
-      <c r="AJ46" s="124"/>
-      <c r="AK46" s="124"/>
-      <c r="AL46" s="124"/>
-      <c r="AM46" s="139" t="s">
+      <c r="T46" s="107"/>
+      <c r="U46" s="107"/>
+      <c r="V46" s="107"/>
+      <c r="W46" s="107"/>
+      <c r="X46" s="107"/>
+      <c r="Y46" s="107"/>
+      <c r="Z46" s="107"/>
+      <c r="AA46" s="107"/>
+      <c r="AB46" s="107"/>
+      <c r="AC46" s="107"/>
+      <c r="AD46" s="107"/>
+      <c r="AE46" s="107"/>
+      <c r="AF46" s="107"/>
+      <c r="AG46" s="107"/>
+      <c r="AH46" s="107"/>
+      <c r="AI46" s="107"/>
+      <c r="AJ46" s="107"/>
+      <c r="AK46" s="107"/>
+      <c r="AL46" s="107"/>
+      <c r="AM46" s="122" t="s">
         <v>1409</v>
       </c>
-      <c r="AN46" s="124"/>
-      <c r="AO46" s="124"/>
-      <c r="AP46" s="124"/>
-      <c r="AQ46" s="124"/>
-      <c r="AR46" s="124"/>
-      <c r="AS46" s="124"/>
-      <c r="AT46" s="124"/>
-      <c r="AU46" s="124"/>
-      <c r="AV46" s="124"/>
-      <c r="AW46" s="124"/>
-      <c r="AX46" s="124"/>
-      <c r="AY46" s="124"/>
-      <c r="AZ46" s="124"/>
-      <c r="BA46" s="124"/>
-      <c r="BB46" s="124"/>
-      <c r="BC46" s="124"/>
-      <c r="BD46" s="124"/>
-      <c r="BE46" s="124"/>
-      <c r="BF46" s="124"/>
-      <c r="BG46" s="124"/>
-      <c r="BH46" s="124"/>
-      <c r="BI46" s="124"/>
-      <c r="BJ46" s="124"/>
-      <c r="BK46" s="124"/>
-      <c r="BL46" s="124"/>
-      <c r="BM46" s="124"/>
-      <c r="BN46" s="124"/>
-      <c r="BO46" s="124"/>
-      <c r="BP46" s="124"/>
-      <c r="BQ46" s="124"/>
-      <c r="BR46" s="125"/>
+      <c r="AN46" s="107"/>
+      <c r="AO46" s="107"/>
+      <c r="AP46" s="107"/>
+      <c r="AQ46" s="107"/>
+      <c r="AR46" s="107"/>
+      <c r="AS46" s="107"/>
+      <c r="AT46" s="107"/>
+      <c r="AU46" s="107"/>
+      <c r="AV46" s="107"/>
+      <c r="AW46" s="107"/>
+      <c r="AX46" s="107"/>
+      <c r="AY46" s="107"/>
+      <c r="AZ46" s="107"/>
+      <c r="BA46" s="107"/>
+      <c r="BB46" s="107"/>
+      <c r="BC46" s="107"/>
+      <c r="BD46" s="107"/>
+      <c r="BE46" s="107"/>
+      <c r="BF46" s="107"/>
+      <c r="BG46" s="107"/>
+      <c r="BH46" s="107"/>
+      <c r="BI46" s="107"/>
+      <c r="BJ46" s="107"/>
+      <c r="BK46" s="107"/>
+      <c r="BL46" s="107"/>
+      <c r="BM46" s="107"/>
+      <c r="BN46" s="107"/>
+      <c r="BO46" s="107"/>
+      <c r="BP46" s="107"/>
+      <c r="BQ46" s="107"/>
+      <c r="BR46" s="108"/>
     </row>
     <row r="47" spans="1:70" ht="15" thickTop="1">
-      <c r="A47" s="141"/>
-      <c r="E47" s="134" t="s">
+      <c r="A47" s="124"/>
+      <c r="E47" s="117" t="s">
         <v>1410</v>
       </c>
-      <c r="F47" s="135"/>
-      <c r="G47" s="135"/>
-      <c r="H47" s="137" t="s">
+      <c r="F47" s="118"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="120" t="s">
         <v>1411</v>
       </c>
-      <c r="I47" s="135"/>
-      <c r="J47" s="135"/>
-      <c r="K47" s="135"/>
-      <c r="L47" s="135"/>
-      <c r="M47" s="135"/>
-      <c r="N47" s="135"/>
-      <c r="O47" s="135"/>
-      <c r="P47" s="135"/>
-      <c r="Q47" s="135"/>
-      <c r="R47" s="136"/>
-      <c r="S47" s="160" t="s">
+      <c r="I47" s="118"/>
+      <c r="J47" s="118"/>
+      <c r="K47" s="118"/>
+      <c r="L47" s="118"/>
+      <c r="M47" s="118"/>
+      <c r="N47" s="118"/>
+      <c r="O47" s="118"/>
+      <c r="P47" s="118"/>
+      <c r="Q47" s="118"/>
+      <c r="R47" s="119"/>
+      <c r="S47" s="143" t="s">
         <v>1412</v>
       </c>
-      <c r="T47" s="135"/>
-      <c r="U47" s="135"/>
-      <c r="V47" s="135"/>
-      <c r="W47" s="135"/>
-      <c r="X47" s="135"/>
-      <c r="Y47" s="135"/>
-      <c r="Z47" s="135"/>
-      <c r="AA47" s="135"/>
-      <c r="AB47" s="135"/>
-      <c r="AC47" s="135"/>
-      <c r="AD47" s="135"/>
-      <c r="AE47" s="135"/>
-      <c r="AF47" s="135"/>
-      <c r="AG47" s="135"/>
-      <c r="AH47" s="135"/>
-      <c r="AI47" s="135"/>
-      <c r="AJ47" s="135"/>
-      <c r="AK47" s="135"/>
-      <c r="AL47" s="135"/>
-      <c r="AM47" s="161" t="s">
+      <c r="T47" s="118"/>
+      <c r="U47" s="118"/>
+      <c r="V47" s="118"/>
+      <c r="W47" s="118"/>
+      <c r="X47" s="118"/>
+      <c r="Y47" s="118"/>
+      <c r="Z47" s="118"/>
+      <c r="AA47" s="118"/>
+      <c r="AB47" s="118"/>
+      <c r="AC47" s="118"/>
+      <c r="AD47" s="118"/>
+      <c r="AE47" s="118"/>
+      <c r="AF47" s="118"/>
+      <c r="AG47" s="118"/>
+      <c r="AH47" s="118"/>
+      <c r="AI47" s="118"/>
+      <c r="AJ47" s="118"/>
+      <c r="AK47" s="118"/>
+      <c r="AL47" s="118"/>
+      <c r="AM47" s="144" t="s">
         <v>1413</v>
       </c>
-      <c r="AN47" s="135"/>
-      <c r="AO47" s="135"/>
-      <c r="AP47" s="135"/>
-      <c r="AQ47" s="135"/>
-      <c r="AR47" s="135"/>
-      <c r="AS47" s="135"/>
-      <c r="AT47" s="135"/>
-      <c r="AU47" s="135"/>
-      <c r="AV47" s="135"/>
-      <c r="AW47" s="135"/>
-      <c r="AX47" s="135"/>
-      <c r="AY47" s="135"/>
-      <c r="AZ47" s="135"/>
-      <c r="BA47" s="135"/>
-      <c r="BB47" s="135"/>
-      <c r="BC47" s="135"/>
-      <c r="BD47" s="135"/>
-      <c r="BE47" s="135"/>
-      <c r="BF47" s="135"/>
-      <c r="BG47" s="135"/>
-      <c r="BH47" s="135"/>
-      <c r="BI47" s="135"/>
-      <c r="BJ47" s="135"/>
-      <c r="BK47" s="135"/>
-      <c r="BL47" s="135"/>
-      <c r="BM47" s="135"/>
-      <c r="BN47" s="135"/>
-      <c r="BO47" s="135"/>
-      <c r="BP47" s="135"/>
-      <c r="BQ47" s="135"/>
-      <c r="BR47" s="136"/>
+      <c r="AN47" s="118"/>
+      <c r="AO47" s="118"/>
+      <c r="AP47" s="118"/>
+      <c r="AQ47" s="118"/>
+      <c r="AR47" s="118"/>
+      <c r="AS47" s="118"/>
+      <c r="AT47" s="118"/>
+      <c r="AU47" s="118"/>
+      <c r="AV47" s="118"/>
+      <c r="AW47" s="118"/>
+      <c r="AX47" s="118"/>
+      <c r="AY47" s="118"/>
+      <c r="AZ47" s="118"/>
+      <c r="BA47" s="118"/>
+      <c r="BB47" s="118"/>
+      <c r="BC47" s="118"/>
+      <c r="BD47" s="118"/>
+      <c r="BE47" s="118"/>
+      <c r="BF47" s="118"/>
+      <c r="BG47" s="118"/>
+      <c r="BH47" s="118"/>
+      <c r="BI47" s="118"/>
+      <c r="BJ47" s="118"/>
+      <c r="BK47" s="118"/>
+      <c r="BL47" s="118"/>
+      <c r="BM47" s="118"/>
+      <c r="BN47" s="118"/>
+      <c r="BO47" s="118"/>
+      <c r="BP47" s="118"/>
+      <c r="BQ47" s="118"/>
+      <c r="BR47" s="119"/>
     </row>
     <row r="48" spans="1:70">
-      <c r="A48" s="141"/>
-      <c r="E48" s="126" t="s">
+      <c r="A48" s="124"/>
+      <c r="E48" s="109" t="s">
         <v>1414</v>
       </c>
-      <c r="F48" s="127"/>
-      <c r="G48" s="127"/>
-      <c r="H48" s="129" t="s">
+      <c r="F48" s="110"/>
+      <c r="G48" s="110"/>
+      <c r="H48" s="112" t="s">
         <v>1415</v>
       </c>
-      <c r="I48" s="127"/>
-      <c r="J48" s="127"/>
-      <c r="K48" s="127"/>
-      <c r="L48" s="127"/>
-      <c r="M48" s="127"/>
-      <c r="N48" s="127"/>
-      <c r="O48" s="127"/>
-      <c r="P48" s="127"/>
-      <c r="Q48" s="127"/>
-      <c r="R48" s="128"/>
-      <c r="S48" s="162" t="s">
+      <c r="I48" s="110"/>
+      <c r="J48" s="110"/>
+      <c r="K48" s="110"/>
+      <c r="L48" s="110"/>
+      <c r="M48" s="110"/>
+      <c r="N48" s="110"/>
+      <c r="O48" s="110"/>
+      <c r="P48" s="110"/>
+      <c r="Q48" s="110"/>
+      <c r="R48" s="111"/>
+      <c r="S48" s="145" t="s">
         <v>1416</v>
       </c>
-      <c r="T48" s="127"/>
-      <c r="U48" s="127"/>
-      <c r="V48" s="127"/>
-      <c r="W48" s="127"/>
-      <c r="X48" s="127"/>
-      <c r="Y48" s="127"/>
-      <c r="Z48" s="127"/>
-      <c r="AA48" s="127"/>
-      <c r="AB48" s="127"/>
-      <c r="AC48" s="127"/>
-      <c r="AD48" s="127"/>
-      <c r="AE48" s="127"/>
-      <c r="AF48" s="127"/>
-      <c r="AG48" s="127"/>
-      <c r="AH48" s="127"/>
-      <c r="AI48" s="127"/>
-      <c r="AJ48" s="127"/>
-      <c r="AK48" s="127"/>
-      <c r="AL48" s="127"/>
-      <c r="AM48" s="138" t="s">
+      <c r="T48" s="110"/>
+      <c r="U48" s="110"/>
+      <c r="V48" s="110"/>
+      <c r="W48" s="110"/>
+      <c r="X48" s="110"/>
+      <c r="Y48" s="110"/>
+      <c r="Z48" s="110"/>
+      <c r="AA48" s="110"/>
+      <c r="AB48" s="110"/>
+      <c r="AC48" s="110"/>
+      <c r="AD48" s="110"/>
+      <c r="AE48" s="110"/>
+      <c r="AF48" s="110"/>
+      <c r="AG48" s="110"/>
+      <c r="AH48" s="110"/>
+      <c r="AI48" s="110"/>
+      <c r="AJ48" s="110"/>
+      <c r="AK48" s="110"/>
+      <c r="AL48" s="110"/>
+      <c r="AM48" s="121" t="s">
         <v>1417</v>
       </c>
-      <c r="AN48" s="127"/>
-      <c r="AO48" s="127"/>
-      <c r="AP48" s="127"/>
-      <c r="AQ48" s="127"/>
-      <c r="AR48" s="127"/>
-      <c r="AS48" s="127"/>
-      <c r="AT48" s="127"/>
-      <c r="AU48" s="127"/>
-      <c r="AV48" s="127"/>
-      <c r="AW48" s="127"/>
-      <c r="AX48" s="127"/>
-      <c r="AY48" s="127"/>
-      <c r="AZ48" s="127"/>
-      <c r="BA48" s="127"/>
-      <c r="BB48" s="127"/>
-      <c r="BC48" s="127"/>
-      <c r="BD48" s="127"/>
-      <c r="BE48" s="127"/>
-      <c r="BF48" s="127"/>
-      <c r="BG48" s="127"/>
-      <c r="BH48" s="127"/>
-      <c r="BI48" s="127"/>
-      <c r="BJ48" s="127"/>
-      <c r="BK48" s="127"/>
-      <c r="BL48" s="127"/>
-      <c r="BM48" s="127"/>
-      <c r="BN48" s="127"/>
-      <c r="BO48" s="127"/>
-      <c r="BP48" s="127"/>
-      <c r="BQ48" s="127"/>
-      <c r="BR48" s="128"/>
+      <c r="AN48" s="110"/>
+      <c r="AO48" s="110"/>
+      <c r="AP48" s="110"/>
+      <c r="AQ48" s="110"/>
+      <c r="AR48" s="110"/>
+      <c r="AS48" s="110"/>
+      <c r="AT48" s="110"/>
+      <c r="AU48" s="110"/>
+      <c r="AV48" s="110"/>
+      <c r="AW48" s="110"/>
+      <c r="AX48" s="110"/>
+      <c r="AY48" s="110"/>
+      <c r="AZ48" s="110"/>
+      <c r="BA48" s="110"/>
+      <c r="BB48" s="110"/>
+      <c r="BC48" s="110"/>
+      <c r="BD48" s="110"/>
+      <c r="BE48" s="110"/>
+      <c r="BF48" s="110"/>
+      <c r="BG48" s="110"/>
+      <c r="BH48" s="110"/>
+      <c r="BI48" s="110"/>
+      <c r="BJ48" s="110"/>
+      <c r="BK48" s="110"/>
+      <c r="BL48" s="110"/>
+      <c r="BM48" s="110"/>
+      <c r="BN48" s="110"/>
+      <c r="BO48" s="110"/>
+      <c r="BP48" s="110"/>
+      <c r="BQ48" s="110"/>
+      <c r="BR48" s="111"/>
     </row>
     <row r="49" spans="1:70">
-      <c r="A49" s="141"/>
-      <c r="E49" s="163" t="s">
+      <c r="A49" s="124"/>
+      <c r="E49" s="146" t="s">
         <v>1418</v>
       </c>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="133" t="s">
+      <c r="F49" s="114"/>
+      <c r="G49" s="114"/>
+      <c r="H49" s="116" t="s">
         <v>1419</v>
       </c>
-      <c r="I49" s="131"/>
-      <c r="J49" s="131"/>
-      <c r="K49" s="131"/>
-      <c r="L49" s="131"/>
-      <c r="M49" s="131"/>
-      <c r="N49" s="131"/>
-      <c r="O49" s="131"/>
-      <c r="P49" s="131"/>
-      <c r="Q49" s="131"/>
-      <c r="R49" s="132"/>
-      <c r="S49" s="164" t="s">
+      <c r="I49" s="114"/>
+      <c r="J49" s="114"/>
+      <c r="K49" s="114"/>
+      <c r="L49" s="114"/>
+      <c r="M49" s="114"/>
+      <c r="N49" s="114"/>
+      <c r="O49" s="114"/>
+      <c r="P49" s="114"/>
+      <c r="Q49" s="114"/>
+      <c r="R49" s="115"/>
+      <c r="S49" s="147" t="s">
         <v>1420</v>
       </c>
-      <c r="T49" s="131"/>
-      <c r="U49" s="131"/>
-      <c r="V49" s="131"/>
-      <c r="W49" s="131"/>
-      <c r="X49" s="131"/>
-      <c r="Y49" s="131"/>
-      <c r="Z49" s="131"/>
-      <c r="AA49" s="131"/>
-      <c r="AB49" s="131"/>
-      <c r="AC49" s="131"/>
-      <c r="AD49" s="131"/>
-      <c r="AE49" s="131"/>
-      <c r="AF49" s="131"/>
-      <c r="AG49" s="131"/>
-      <c r="AH49" s="131"/>
-      <c r="AI49" s="131"/>
-      <c r="AJ49" s="131"/>
-      <c r="AK49" s="131"/>
-      <c r="AL49" s="131"/>
-      <c r="AM49" s="165" t="s">
+      <c r="T49" s="114"/>
+      <c r="U49" s="114"/>
+      <c r="V49" s="114"/>
+      <c r="W49" s="114"/>
+      <c r="X49" s="114"/>
+      <c r="Y49" s="114"/>
+      <c r="Z49" s="114"/>
+      <c r="AA49" s="114"/>
+      <c r="AB49" s="114"/>
+      <c r="AC49" s="114"/>
+      <c r="AD49" s="114"/>
+      <c r="AE49" s="114"/>
+      <c r="AF49" s="114"/>
+      <c r="AG49" s="114"/>
+      <c r="AH49" s="114"/>
+      <c r="AI49" s="114"/>
+      <c r="AJ49" s="114"/>
+      <c r="AK49" s="114"/>
+      <c r="AL49" s="114"/>
+      <c r="AM49" s="148" t="s">
         <v>1421</v>
       </c>
-      <c r="AN49" s="131"/>
-      <c r="AO49" s="131"/>
-      <c r="AP49" s="131"/>
-      <c r="AQ49" s="131"/>
-      <c r="AR49" s="131"/>
-      <c r="AS49" s="131"/>
-      <c r="AT49" s="131"/>
-      <c r="AU49" s="131"/>
-      <c r="AV49" s="131"/>
-      <c r="AW49" s="131"/>
-      <c r="AX49" s="131"/>
-      <c r="AY49" s="131"/>
-      <c r="AZ49" s="131"/>
-      <c r="BA49" s="131"/>
-      <c r="BB49" s="131"/>
-      <c r="BC49" s="131"/>
-      <c r="BD49" s="131"/>
-      <c r="BE49" s="131"/>
-      <c r="BF49" s="131"/>
-      <c r="BG49" s="131"/>
-      <c r="BH49" s="131"/>
-      <c r="BI49" s="131"/>
-      <c r="BJ49" s="131"/>
-      <c r="BK49" s="131"/>
-      <c r="BL49" s="131"/>
-      <c r="BM49" s="131"/>
-      <c r="BN49" s="131"/>
-      <c r="BO49" s="131"/>
-      <c r="BP49" s="131"/>
-      <c r="BQ49" s="131"/>
-      <c r="BR49" s="132"/>
+      <c r="AN49" s="114"/>
+      <c r="AO49" s="114"/>
+      <c r="AP49" s="114"/>
+      <c r="AQ49" s="114"/>
+      <c r="AR49" s="114"/>
+      <c r="AS49" s="114"/>
+      <c r="AT49" s="114"/>
+      <c r="AU49" s="114"/>
+      <c r="AV49" s="114"/>
+      <c r="AW49" s="114"/>
+      <c r="AX49" s="114"/>
+      <c r="AY49" s="114"/>
+      <c r="AZ49" s="114"/>
+      <c r="BA49" s="114"/>
+      <c r="BB49" s="114"/>
+      <c r="BC49" s="114"/>
+      <c r="BD49" s="114"/>
+      <c r="BE49" s="114"/>
+      <c r="BF49" s="114"/>
+      <c r="BG49" s="114"/>
+      <c r="BH49" s="114"/>
+      <c r="BI49" s="114"/>
+      <c r="BJ49" s="114"/>
+      <c r="BK49" s="114"/>
+      <c r="BL49" s="114"/>
+      <c r="BM49" s="114"/>
+      <c r="BN49" s="114"/>
+      <c r="BO49" s="114"/>
+      <c r="BP49" s="114"/>
+      <c r="BQ49" s="114"/>
+      <c r="BR49" s="115"/>
     </row>
     <row r="50" spans="1:70">
-      <c r="A50" s="141"/>
-      <c r="E50" s="126" t="s">
+      <c r="A50" s="124"/>
+      <c r="E50" s="109" t="s">
         <v>1422</v>
       </c>
-      <c r="F50" s="127"/>
-      <c r="G50" s="127"/>
-      <c r="H50" s="129" t="s">
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="112" t="s">
         <v>1423</v>
       </c>
-      <c r="I50" s="127"/>
-      <c r="J50" s="127"/>
-      <c r="K50" s="127"/>
-      <c r="L50" s="127"/>
-      <c r="M50" s="127"/>
-      <c r="N50" s="127"/>
-      <c r="O50" s="127"/>
-      <c r="P50" s="127"/>
-      <c r="Q50" s="127"/>
-      <c r="R50" s="128"/>
-      <c r="S50" s="162" t="s">
+      <c r="I50" s="110"/>
+      <c r="J50" s="110"/>
+      <c r="K50" s="110"/>
+      <c r="L50" s="110"/>
+      <c r="M50" s="110"/>
+      <c r="N50" s="110"/>
+      <c r="O50" s="110"/>
+      <c r="P50" s="110"/>
+      <c r="Q50" s="110"/>
+      <c r="R50" s="111"/>
+      <c r="S50" s="145" t="s">
         <v>1424</v>
       </c>
-      <c r="T50" s="127"/>
-      <c r="U50" s="127"/>
-      <c r="V50" s="127"/>
-      <c r="W50" s="127"/>
-      <c r="X50" s="127"/>
-      <c r="Y50" s="127"/>
-      <c r="Z50" s="127"/>
-      <c r="AA50" s="127"/>
-      <c r="AB50" s="127"/>
-      <c r="AC50" s="127"/>
-      <c r="AD50" s="127"/>
-      <c r="AE50" s="127"/>
-      <c r="AF50" s="127"/>
-      <c r="AG50" s="127"/>
-      <c r="AH50" s="127"/>
-      <c r="AI50" s="127"/>
-      <c r="AJ50" s="127"/>
-      <c r="AK50" s="127"/>
-      <c r="AL50" s="127"/>
-      <c r="AM50" s="166" t="s">
+      <c r="T50" s="110"/>
+      <c r="U50" s="110"/>
+      <c r="V50" s="110"/>
+      <c r="W50" s="110"/>
+      <c r="X50" s="110"/>
+      <c r="Y50" s="110"/>
+      <c r="Z50" s="110"/>
+      <c r="AA50" s="110"/>
+      <c r="AB50" s="110"/>
+      <c r="AC50" s="110"/>
+      <c r="AD50" s="110"/>
+      <c r="AE50" s="110"/>
+      <c r="AF50" s="110"/>
+      <c r="AG50" s="110"/>
+      <c r="AH50" s="110"/>
+      <c r="AI50" s="110"/>
+      <c r="AJ50" s="110"/>
+      <c r="AK50" s="110"/>
+      <c r="AL50" s="110"/>
+      <c r="AM50" s="149" t="s">
         <v>1425</v>
       </c>
-      <c r="AN50" s="127"/>
-      <c r="AO50" s="127"/>
-      <c r="AP50" s="127"/>
-      <c r="AQ50" s="127"/>
-      <c r="AR50" s="127"/>
-      <c r="AS50" s="127"/>
-      <c r="AT50" s="127"/>
-      <c r="AU50" s="127"/>
-      <c r="AV50" s="127"/>
-      <c r="AW50" s="127"/>
-      <c r="AX50" s="127"/>
-      <c r="AY50" s="127"/>
-      <c r="AZ50" s="127"/>
-      <c r="BA50" s="127"/>
-      <c r="BB50" s="127"/>
-      <c r="BC50" s="127"/>
-      <c r="BD50" s="127"/>
-      <c r="BE50" s="127"/>
-      <c r="BF50" s="127"/>
-      <c r="BG50" s="127"/>
-      <c r="BH50" s="127"/>
-      <c r="BI50" s="127"/>
-      <c r="BJ50" s="127"/>
-      <c r="BK50" s="127"/>
-      <c r="BL50" s="127"/>
-      <c r="BM50" s="127"/>
-      <c r="BN50" s="127"/>
-      <c r="BO50" s="127"/>
-      <c r="BP50" s="127"/>
-      <c r="BQ50" s="127"/>
-      <c r="BR50" s="128"/>
+      <c r="AN50" s="110"/>
+      <c r="AO50" s="110"/>
+      <c r="AP50" s="110"/>
+      <c r="AQ50" s="110"/>
+      <c r="AR50" s="110"/>
+      <c r="AS50" s="110"/>
+      <c r="AT50" s="110"/>
+      <c r="AU50" s="110"/>
+      <c r="AV50" s="110"/>
+      <c r="AW50" s="110"/>
+      <c r="AX50" s="110"/>
+      <c r="AY50" s="110"/>
+      <c r="AZ50" s="110"/>
+      <c r="BA50" s="110"/>
+      <c r="BB50" s="110"/>
+      <c r="BC50" s="110"/>
+      <c r="BD50" s="110"/>
+      <c r="BE50" s="110"/>
+      <c r="BF50" s="110"/>
+      <c r="BG50" s="110"/>
+      <c r="BH50" s="110"/>
+      <c r="BI50" s="110"/>
+      <c r="BJ50" s="110"/>
+      <c r="BK50" s="110"/>
+      <c r="BL50" s="110"/>
+      <c r="BM50" s="110"/>
+      <c r="BN50" s="110"/>
+      <c r="BO50" s="110"/>
+      <c r="BP50" s="110"/>
+      <c r="BQ50" s="110"/>
+      <c r="BR50" s="111"/>
     </row>
     <row r="51" spans="1:70">
-      <c r="A51" s="141"/>
-      <c r="E51" s="163" t="s">
+      <c r="A51" s="124"/>
+      <c r="E51" s="146" t="s">
         <v>1426</v>
       </c>
-      <c r="F51" s="131"/>
-      <c r="G51" s="131"/>
-      <c r="H51" s="133" t="s">
+      <c r="F51" s="114"/>
+      <c r="G51" s="114"/>
+      <c r="H51" s="116" t="s">
         <v>1427</v>
       </c>
-      <c r="I51" s="131"/>
-      <c r="J51" s="131"/>
-      <c r="K51" s="131"/>
-      <c r="L51" s="131"/>
-      <c r="M51" s="131"/>
-      <c r="N51" s="131"/>
-      <c r="O51" s="131"/>
-      <c r="P51" s="131"/>
-      <c r="Q51" s="131"/>
-      <c r="R51" s="132"/>
-      <c r="S51" s="164" t="s">
+      <c r="I51" s="114"/>
+      <c r="J51" s="114"/>
+      <c r="K51" s="114"/>
+      <c r="L51" s="114"/>
+      <c r="M51" s="114"/>
+      <c r="N51" s="114"/>
+      <c r="O51" s="114"/>
+      <c r="P51" s="114"/>
+      <c r="Q51" s="114"/>
+      <c r="R51" s="115"/>
+      <c r="S51" s="147" t="s">
         <v>1428</v>
       </c>
-      <c r="T51" s="131"/>
-      <c r="U51" s="131"/>
-      <c r="V51" s="131"/>
-      <c r="W51" s="131"/>
-      <c r="X51" s="131"/>
-      <c r="Y51" s="131"/>
-      <c r="Z51" s="131"/>
-      <c r="AA51" s="131"/>
-      <c r="AB51" s="131"/>
-      <c r="AC51" s="131"/>
-      <c r="AD51" s="131"/>
-      <c r="AE51" s="131"/>
-      <c r="AF51" s="131"/>
-      <c r="AG51" s="131"/>
-      <c r="AH51" s="131"/>
-      <c r="AI51" s="131"/>
-      <c r="AJ51" s="131"/>
-      <c r="AK51" s="131"/>
-      <c r="AL51" s="131"/>
-      <c r="AM51" s="165" t="s">
+      <c r="T51" s="114"/>
+      <c r="U51" s="114"/>
+      <c r="V51" s="114"/>
+      <c r="W51" s="114"/>
+      <c r="X51" s="114"/>
+      <c r="Y51" s="114"/>
+      <c r="Z51" s="114"/>
+      <c r="AA51" s="114"/>
+      <c r="AB51" s="114"/>
+      <c r="AC51" s="114"/>
+      <c r="AD51" s="114"/>
+      <c r="AE51" s="114"/>
+      <c r="AF51" s="114"/>
+      <c r="AG51" s="114"/>
+      <c r="AH51" s="114"/>
+      <c r="AI51" s="114"/>
+      <c r="AJ51" s="114"/>
+      <c r="AK51" s="114"/>
+      <c r="AL51" s="114"/>
+      <c r="AM51" s="148" t="s">
         <v>1429</v>
       </c>
-      <c r="AN51" s="131"/>
-      <c r="AO51" s="131"/>
-      <c r="AP51" s="131"/>
-      <c r="AQ51" s="131"/>
-      <c r="AR51" s="131"/>
-      <c r="AS51" s="131"/>
-      <c r="AT51" s="131"/>
-      <c r="AU51" s="131"/>
-      <c r="AV51" s="131"/>
-      <c r="AW51" s="131"/>
-      <c r="AX51" s="131"/>
-      <c r="AY51" s="131"/>
-      <c r="AZ51" s="131"/>
-      <c r="BA51" s="131"/>
-      <c r="BB51" s="131"/>
-      <c r="BC51" s="131"/>
-      <c r="BD51" s="131"/>
-      <c r="BE51" s="131"/>
-      <c r="BF51" s="131"/>
-      <c r="BG51" s="131"/>
-      <c r="BH51" s="131"/>
-      <c r="BI51" s="131"/>
-      <c r="BJ51" s="131"/>
-      <c r="BK51" s="131"/>
-      <c r="BL51" s="131"/>
-      <c r="BM51" s="131"/>
-      <c r="BN51" s="131"/>
-      <c r="BO51" s="131"/>
-      <c r="BP51" s="131"/>
-      <c r="BQ51" s="131"/>
-      <c r="BR51" s="132"/>
+      <c r="AN51" s="114"/>
+      <c r="AO51" s="114"/>
+      <c r="AP51" s="114"/>
+      <c r="AQ51" s="114"/>
+      <c r="AR51" s="114"/>
+      <c r="AS51" s="114"/>
+      <c r="AT51" s="114"/>
+      <c r="AU51" s="114"/>
+      <c r="AV51" s="114"/>
+      <c r="AW51" s="114"/>
+      <c r="AX51" s="114"/>
+      <c r="AY51" s="114"/>
+      <c r="AZ51" s="114"/>
+      <c r="BA51" s="114"/>
+      <c r="BB51" s="114"/>
+      <c r="BC51" s="114"/>
+      <c r="BD51" s="114"/>
+      <c r="BE51" s="114"/>
+      <c r="BF51" s="114"/>
+      <c r="BG51" s="114"/>
+      <c r="BH51" s="114"/>
+      <c r="BI51" s="114"/>
+      <c r="BJ51" s="114"/>
+      <c r="BK51" s="114"/>
+      <c r="BL51" s="114"/>
+      <c r="BM51" s="114"/>
+      <c r="BN51" s="114"/>
+      <c r="BO51" s="114"/>
+      <c r="BP51" s="114"/>
+      <c r="BQ51" s="114"/>
+      <c r="BR51" s="115"/>
     </row>
     <row r="53" spans="1:70">
-      <c r="E53" s="148" t="s">
+      <c r="E53" s="131" t="s">
         <v>1430</v>
       </c>
     </row>
@@ -20299,13 +20299,13 @@
       </c>
     </row>
     <row r="156" spans="1:6">
-      <c r="A156" s="116" t="s">
+      <c r="A156" s="165" t="s">
         <v>619</v>
       </c>
-      <c r="B156" s="116"/>
-      <c r="C156" s="116"/>
-      <c r="D156" s="116"/>
-      <c r="E156" s="116"/>
+      <c r="B156" s="165"/>
+      <c r="C156" s="165"/>
+      <c r="D156" s="165"/>
+      <c r="E156" s="165"/>
       <c r="F156" s="36"/>
     </row>
     <row r="157" spans="1:6">
@@ -20432,13 +20432,13 @@
       </c>
     </row>
     <row r="187" spans="1:6">
-      <c r="A187" s="116" t="s">
+      <c r="A187" s="165" t="s">
         <v>642</v>
       </c>
-      <c r="B187" s="116"/>
-      <c r="C187" s="116"/>
-      <c r="D187" s="116"/>
-      <c r="E187" s="116"/>
+      <c r="B187" s="165"/>
+      <c r="C187" s="165"/>
+      <c r="D187" s="165"/>
+      <c r="E187" s="165"/>
       <c r="F187" s="36"/>
     </row>
     <row r="188" spans="1:6">

</xml_diff>